<commit_message>
Adds javascript formatting for team
</commit_message>
<xml_diff>
--- a/data/1QB_Predraft_Rookies.xlsx
+++ b/data/1QB_Predraft_Rookies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE842B45-317F-4E4E-9F71-D1A55C002241}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86B36148-9C76-469B-9220-75EDF344A8CB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="38020" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
+    <workbookView xWindow="0" yWindow="22690" windowWidth="21590" windowHeight="15110" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="127">
   <si>
     <t>Rk</t>
   </si>
@@ -381,6 +381,89 @@
   </si>
   <si>
     <t>Isiah Pacheco, Jaylen Wright, Ty Johnson</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tetairoa McMillan is an early-declare wide receiver with a lot of size, who gave Arizona solid production.   
+His Breakout Score is good, but not amazing, sitting at 83.1. His raw numbers in yards per team attempt were good, but they were brought down a bit when adjusted for the strength of the opponent.   
+His comparisons to Drake London don’t work well analytically, as London had a much better age-adjusted profile. London's Breakout Score was elite. Profiles like Tee Higgins and Courtland Sutton make a lot more sense. They didn’t get the draft capital McMillan is likely to get, but their fantasy impacts have definitely been felt.   
+</t>
+  </si>
+  <si>
+    <t>Ashton Jeanty’s early ZAP score is 99.2. If it remains above 99, he’ll join a small group of running backs to achieve that score.    
+He is described as being as good as it gets, with the size to handle a large workload. His best season in prorated reception share is sixth-best in the ZAP model’s history, and his Breakout Score is 94.3.    
+He is one of six players in the model’s database to have a best season total yards per team play above 2.8. There is a possibility that Boise State’s strength of schedule inflated Jeanty’s numbers, but that will be reflected in his draft capital.    
+Finding statistical comparisons for Jeanty is difficult, as there hasn’t been a prospect like him since 2011.    
+Sources and related content</t>
+  </si>
+  <si>
+    <t>Omarion Hampton is a running back from North Carolina. His Breakout Score of 61.7 is slightly below average in this running back class. His top-season reception share is 17.9%, which is third-best in the class. He had a prorated total yards per team play rate last season of 2.48. That was also top-3 among combine invites. He weighs 221 pounds and ran a 4.46 40-yard dash</t>
+  </si>
+  <si>
+    <t>The ZAP Model “loves” Luther Burden. His 96.3 Breakout Score is the highest in the class, and his top season in adjusted receiving yards per team pass attempt ranks second. He is an early-declare receiver with one of the best yards-after-catch profiles in the class. He also had rushing production in college.
+Burden ran roughly 83% of his routes from the slot while at Missouri. He only has one great season of production; his sophomore campaign was impressive, but his rates were below 2.0 in his Freshman and Junior seasons. He didn’t do typical wide receiver things during his big Sophomore year.
+Despite this, he has the yards-after-catch and play-making tools to make a huge impact in the NFL. There’s a lot of volatility that the ZAP Model isn’t fully capturing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ZAP Model may not be giving TreVeyon Henderson enough credit for what he did in college.    
+As a Freshman at Ohio State, Henderson ran the ball 183 times for 1,248 yards and 15 touchdowns.  He also caught 27 passes for 312 yards and 4 more touchdowns.    
+That Freshman-season production led to an 86.4 Breakout Score for Henderson, the seventh-best mark in the class.    
+Henderson is getting knocked down a tad in the model because he had a best-season reception share of just 9.7%.  That ranks 20th out of the 31 running backs who were invited to the combine this year.    
+In the ZAP Model database, there’ve only been five running backs with a best-season reception share below 10% and a Breakout Score above 80.    
+Effectively, this is telling us that Henderson was really good once he got the ball in his hands.    
+There may be some questions about his potential ground-game workload at the next level.  Henderson maxed out at 183 rush attempts in a single season at Ohio State.    
+He should be able to use his excellent pass protection skills and efficiency to be a solid PPR asset, at least.    </t>
+  </si>
+  <si>
+    <t>Emeka Egbuka looks like another great wide receiver out of Ohio State. His best collegiate season came in 2022 as a Sophomore, when his prorated receiving yards per team pass attempt rate was 2.81. That was by far the highest of his career, with his second-best season coming in 2024 at 2.22. It’s impressive that Egbuka was able to do that at a young age alongside strong competition.    
+Injuries played a role in the dip from his Sophomore campaign. Egbuka had ankle and knee problems in 2023, so he wasn’t able to keep the momentum going from his wild Sophomore campaign. Then, in 2024, he watched his average depth of target fall to just 7.9, the lowest of his college career. He saw his highest slot rate at 81%.    
+There does seem to be a decent chance that Egbuka plays a slot-only role in the NFL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaleb Johnson played three years at Iowa, but only his final season was really impressive. Since the ZAP Model only takes in receiving inputs, Johnson’s Freshman and Sophomore campaigns are worthless to the model.    
+Things really turned up in 2024. Not only did Johnson carry the ball 240 times for over 1,500 yards, but he also had 22 receptions for 188 yards through the air.  Because of 2024, Johnson registered a Breakout Score of 75.8.    
+Johnson’s 2024 gave him the fourth-highest best-season total yards per team play in the class, and he’s got a top-10 best-season reception share.    
+If there’s a downside with Johnson, it’d probably be that his long speed isn’t as desirable as some of the other top backs in the class. We sort of saw that at the NFL Combine, when he ran his 40-yard dash in 4.57 seconds.    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The rushing portion to Quinshon Judkins’ profile is pretty wild.  As a Freshman at Ole Miss, Judkins ran the ball 274 times for 1,567 yards and 16 scores.  And he did that on a team that had an NFLer in Zach Evans.  After another successful Sophomore year, Judkins decided to chase a national championship at Ohio State for his third and final college season.  And he, alongside running back teammate TreVeyon Henderson, got it.  As impressive as Judkins’ production was throughout college, the ZAP Model isn’t as in love.  Because his receiving numbers weren’t as good.  Judkins had a best-season reception share of 8.6%, a number acquired during his second year at Mississippi.  He ran about 100 fewer routes than Henderson last season, though the two of them finished the year with a nearly identical yards per route run rate.  Judkins Breakout Score was below average, too, at just 46.5.  The class average Breakout Score is 59.4.  I don’t think Judkins is incapable of being a decent receiving threat in the NFL, but there’s a chance we see him and his size focused more on early-down stuff.    
+</t>
+  </si>
+  <si>
+    <t>The ZAP Model has seen nearly 60 wide receivers hit 14 or more PPR points per game in one of their first three seasons in the league.  Just 5 of those 60 did it with a best-season receiving yards per team pass attempt rate below 2.0.  One is Tyreek Hill, who we know is an outlier.  Another is Hunter Renfrow, who only gave us one good year.  The other three are Terry McLaurin, Nico Collins, and Ladd McConkey.    
+Matthew Golden’s best prorated receiving yards per team pass attempt figure was below 2.0.  It was 1.82, done in 2024, his third and final year of college football.  When we adjust for program strength, his top year in yards per team pass attempt is 2.28, not 1.82.  Those team strength adjustments are a key reason Golden’s Breakout Score is an OK-enough 51.4.    
+Golden started his college life at Houston, where he played two seasons and gave us some production.  Receiving yard per team pass attempt rates of 1.38 and 1.32 as a Freshman and Sophomore aren’t tragic.  His top season in yards per route run, per PFF, was 2.10.    
+Golden is probably going to get solid draft capital given his ability to create explosive plays.  He's easy to like on film, and his most favorable comparable in the ZAP Model is Ladd McConkey.  So there are things working in his favor.  He’s just not close to a flawless prospect analytically.</t>
+  </si>
+  <si>
+    <t>When the initial NFL Combine list came out, the Heisman-winning Travis Hunter was only listed as a cornerback. That changed as we got closer to the combine, as he was added to the wide receiver list.  No one really knows how Hunter is going to be used at the next level.  Some believe that he'll be a full-time corner who takes some snaps on offense.  If he's a part-time player on offense, then he'll have a hard time living up to his ZAP score.    
+His production profile is kind of ordinary for a first-rounder.  His top year in receiving yards per team pass attempt came last season, where it was 2.61.  That's a 20th percentile number among all first-round wide receivers since 2011.  His Breakout Score of 66.9 is a 15th percentile one compared to other first-rounders.  His career yards per route run looks slightly better, but, among first-round wide receivers over the last five seasons, it's still below average.  His yards per route run rate was 2.51 last season.  There are 27 wide receivers in this year's class who had a better rate than that during one of their collegiate seasons.    
+We can probably cut Hunter a bit of a break because, you know, he was playing on both offense and defense in college.  None of this is to take away from his insane gifts.  And, to be fair, a lot of evaluators who look solely at film think Hunter is as good as it gets.  If there were no restrictions here -- if we were simply assuming he would play wide receiver -- then I'd more than likely be lower than the market on Hunter.  It's very possible that his metrics aren't showing up well because, again, he did everything for Colorado.  But if we're being completely objective, the predictive metrics we look at aren't close to excellent.</t>
+  </si>
+  <si>
+    <t>No wide receiver in this year's draft class has a higher best-season adjusted receiving yards per team pass attempt than Tre Harris.  Harris' final season at Ole Miss was great.  A 60-catch, 1,030-yard campaign may not look like much, but he amassed that in just eight games.  That led to a (prorated) receiving yards per team pass attempt of 3.86.  Harris' yards per route run last year was even crazier.  According to Pro Football Focus, he saw over five yards per route run.  Not only was that by far the highest in this year's class, but it was the highest PFF has ever recorded from a Power Five wideout with 100 or more routes run.  That dates back to 2014.    
+As impressive as that is, it wasn't all butterflies and rainbows throughout Harris' college career.  He started things off at Louisiana Tech, where he played three seasons.  There, he failed to really break out until his third year.  He then went to Ole Miss where he had back-to-back seasons of strong production, including his ridiculous 2024.    
+We're not usually looking for wide receivers who played five years of college ball.  Younger receivers give us better fantasy football odds.  But, because Harris' numbers were so good at Ole Miss, he ended up with a pretty impressive 83.4 Breakout Score, a top-three number in the class.    
+Older players generally don't have upper-tier Breakout Scores in the model.  Since Breakout Score incorporates age, higher scores tend to correlate with at least average-aged prospects.    
+Harris is an exception.  Especially when you layer on projected draft capital.    
+If Harris gets drafted in the top-100 he's currently forecasted to go in Round 2 then he'll become just the third wideout in ZAP Model history to get picked in the top-100 after turning 23 years old with a Breakout Score above 80. [cite: 4358, 4359, 480.9] The other two?  Sterling Shepard, who had a pretty decent career in the league, and Calvin Ridley.  NFL teams are always looking for perimeter players with decent size.  Harris has that.  And he might be pretty good, too.  He's a higher-variance player to watch.    
+Sources and related content</t>
+  </si>
+  <si>
+    <t>Started playing college football at Alabama.
+Sophomore campaign as a member of the Crimson Tide wasn’t unfortunate.
+Sophomore prorated receiving yards per team pass attempt of 2.06.
+Breakout Score of 77.7, the sixth-highest mark in this year’s class.
+Transferred to Texas, where he played alongside fellow 2025 NFL Combine invite Matthew Golden.
+Was out-produced by Golden.
+Top season in yards per route run was just 2.02.
+Career-long yards per route run was just as bad.
+Gave a little bit of rushing production.
+Showed he was capable of playing both inside and outside of the formation.
+Has elite speed.
+Has a shot in the NFL.</t>
   </si>
 </sst>
 </file>
@@ -758,22 +841,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.82421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.62109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.50390625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.26171875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="8.7421875" style="2"/>
+    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.26953125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="2"/>
+    <col min="11" max="11" width="71.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -804,8 +890,11 @@
       <c r="J1" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="232" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -836,8 +925,11 @@
       <c r="J2" s="2">
         <v>211</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="K2" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -868,8 +960,11 @@
       <c r="J3" s="2">
         <v>221</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -900,8 +995,11 @@
       <c r="J4" s="2">
         <v>219</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="K4" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="174" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -932,8 +1030,11 @@
       <c r="J5" s="2">
         <v>206</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="K5" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="348" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -964,8 +1065,11 @@
       <c r="J6" s="2">
         <v>202</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+      <c r="K6" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="174" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -996,8 +1100,11 @@
       <c r="J7" s="2">
         <v>202</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="K7" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="203" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1028,8 +1135,11 @@
       <c r="J8" s="2">
         <v>224</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="K8" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="203" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1060,8 +1170,11 @@
       <c r="J9" s="2">
         <v>221</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+      <c r="K9" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1092,8 +1205,11 @@
       <c r="J10" s="2">
         <v>191</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1110,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="348" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1141,8 +1257,11 @@
       <c r="J12" s="2">
         <v>188</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+      <c r="K12" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1173,8 +1292,11 @@
       <c r="J13" s="2">
         <v>205</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1191,7 +1313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1223,7 +1345,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1255,7 +1377,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1286,8 +1408,11 @@
       <c r="J17" s="2">
         <v>180</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="K17" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1319,7 +1444,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1351,7 +1476,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1368,7 +1493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1400,7 +1525,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1432,7 +1557,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1449,7 +1574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1481,7 +1606,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1498,7 +1623,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1530,7 +1655,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1562,7 +1687,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1594,7 +1719,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1626,7 +1751,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1658,7 +1783,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1690,7 +1815,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1707,7 +1832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1724,7 +1849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1756,7 +1881,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1788,7 +1913,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1820,7 +1945,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1837,7 +1962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1869,7 +1994,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1901,7 +2026,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1933,7 +2058,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1965,7 +2090,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1997,7 +2122,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2029,7 +2154,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2061,7 +2186,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2093,7 +2218,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2110,7 +2235,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2142,7 +2267,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2174,7 +2299,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Adds Rookie Rankings page
</commit_message>
<xml_diff>
--- a/data/1QB_Predraft_Rookies.xlsx
+++ b/data/1QB_Predraft_Rookies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86B36148-9C76-469B-9220-75EDF344A8CB}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4472E12-1CE1-41B6-BF5E-9B30302E5F45}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="22690" windowWidth="21590" windowHeight="15110" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="38020" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -233,9 +233,6 @@
     <t>DJ Moore, Brandon Aiyuk, Jarvis Landry</t>
   </si>
   <si>
-    <t>Tee Higgins, Courtland Sutto, Mike Williams</t>
-  </si>
-  <si>
     <t>Weekly Starter</t>
   </si>
   <si>
@@ -464,6 +461,9 @@
 Showed he was capable of playing both inside and outside of the formation.
 Has elite speed.
 Has a shot in the NFL.</t>
+  </si>
+  <si>
+    <t>Tee Higgins, Courtland Sutton, Mike Williams</t>
   </si>
 </sst>
 </file>
@@ -522,6 +522,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,10 +845,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -891,10 +896,10 @@
         <v>58</v>
       </c>
       <c r="K1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="232" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="232" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -917,19 +922,19 @@
         <v>62</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="J2" s="2">
         <v>211</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -952,16 +957,16 @@
         <v>62</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" s="2">
         <v>221</v>
       </c>
       <c r="K3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
@@ -987,16 +992,16 @@
         <v>62</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" s="2">
         <v>219</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="174" x14ac:dyDescent="0.35">
@@ -1031,10 +1036,10 @@
         <v>206</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="348" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="348" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1054,19 +1059,19 @@
         <v>91.9</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J6" s="2">
         <v>202</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="174" x14ac:dyDescent="0.35">
@@ -1089,22 +1094,22 @@
         <v>92.8</v>
       </c>
       <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J7" s="2">
         <v>202</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="203" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="203" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1124,22 +1129,22 @@
         <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J8" s="2">
         <v>224</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="203" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="203" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1159,19 +1164,19 @@
         <v>89.5</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J9" s="2">
         <v>221</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
@@ -1194,22 +1199,22 @@
         <v>88.7</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J10" s="2">
         <v>191</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1249,16 +1254,16 @@
         <v>62</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="J12" s="2">
         <v>188</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
@@ -1281,22 +1286,22 @@
         <v>80.900000000000006</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J13" s="2">
         <v>205</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1313,7 +1318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1333,13 +1338,13 @@
         <v>86.9</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="J15" s="2">
         <v>219</v>
@@ -1365,13 +1370,13 @@
         <v>82.7</v>
       </c>
       <c r="G16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="J16" s="2">
         <v>206</v>
@@ -1397,19 +1402,19 @@
         <v>85.3</v>
       </c>
       <c r="G17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J17" s="2">
         <v>180</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1432,19 +1437,19 @@
         <v>81.3</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J18" s="2">
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1464,19 +1469,19 @@
         <v>85.6</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J19" s="2">
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1513,19 +1518,19 @@
         <v>77.3</v>
       </c>
       <c r="G21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="J21" s="2">
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1545,19 +1550,19 @@
         <v>77</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J22" s="2">
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1594,19 +1599,19 @@
         <v>73.5</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J24" s="2">
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1623,7 +1628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1643,13 +1648,13 @@
         <v>81.599999999999994</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J26" s="2">
         <v>200</v>
@@ -1675,19 +1680,19 @@
         <v>77.2</v>
       </c>
       <c r="G27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J27" s="2">
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1707,13 +1712,13 @@
         <v>78.2</v>
       </c>
       <c r="G28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J28" s="2">
         <v>213</v>
@@ -1739,13 +1744,13 @@
         <v>66.3</v>
       </c>
       <c r="G29" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="I29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J29" s="2">
         <v>196</v>
@@ -1771,19 +1776,19 @@
         <v>72.400000000000006</v>
       </c>
       <c r="G30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J30" s="2">
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1803,19 +1808,19 @@
         <v>77.599999999999994</v>
       </c>
       <c r="G31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J31" s="2">
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1832,7 +1837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1849,7 +1854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1869,19 +1874,19 @@
         <v>60.6</v>
       </c>
       <c r="G34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J34" s="2">
         <v>217</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1901,19 +1906,19 @@
         <v>62.5</v>
       </c>
       <c r="G35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J35" s="2">
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1933,19 +1938,19 @@
         <v>46.6</v>
       </c>
       <c r="G36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J36" s="2">
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1962,7 +1967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1982,13 +1987,13 @@
         <v>74.3</v>
       </c>
       <c r="G38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J38" s="2">
         <v>198</v>
@@ -2014,13 +2019,13 @@
         <v>53.5</v>
       </c>
       <c r="G39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J39" s="2">
         <v>184</v>
@@ -2046,19 +2051,19 @@
         <v>76.5</v>
       </c>
       <c r="G40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J40" s="2">
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2078,13 +2083,13 @@
         <v>61.5</v>
       </c>
       <c r="G41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J41" s="2">
         <v>204</v>
@@ -2110,19 +2115,19 @@
         <v>71.3</v>
       </c>
       <c r="G42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J42" s="2">
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2142,19 +2147,19 @@
         <v>65.2</v>
       </c>
       <c r="G43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J43" s="2">
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2174,13 +2179,13 @@
         <v>53.1</v>
       </c>
       <c r="G44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J44" s="2">
         <v>217</v>
@@ -2206,19 +2211,19 @@
         <v>59.3</v>
       </c>
       <c r="G45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J45" s="2">
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2235,7 +2240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2255,13 +2260,13 @@
         <v>46.2</v>
       </c>
       <c r="G47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J47" s="2">
         <v>212</v>
@@ -2287,13 +2292,13 @@
         <v>60</v>
       </c>
       <c r="G48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J48" s="2">
         <v>204</v>
@@ -2319,20 +2324,26 @@
         <v>41.5</v>
       </c>
       <c r="G49" t="s">
+        <v>90</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="I49" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J49" s="2">
         <v>203</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K49" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}"/>
+  <autoFilter ref="A1:K49" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="WR"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates selected formatting, adds additional profiles
</commit_message>
<xml_diff>
--- a/data/1QB_Predraft_Rookies.xlsx
+++ b/data/1QB_Predraft_Rookies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4472E12-1CE1-41B6-BF5E-9B30302E5F45}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14A95A00-27A9-4084-82D9-D804C18F09F6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="38020" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="134">
   <si>
     <t>Rk</t>
   </si>
@@ -387,13 +387,6 @@
 His Breakout Score is good, but not amazing, sitting at 83.1. His raw numbers in yards per team attempt were good, but they were brought down a bit when adjusted for the strength of the opponent.   
 His comparisons to Drake London don’t work well analytically, as London had a much better age-adjusted profile. London's Breakout Score was elite. Profiles like Tee Higgins and Courtland Sutton make a lot more sense. They didn’t get the draft capital McMillan is likely to get, but their fantasy impacts have definitely been felt.   
 </t>
-  </si>
-  <si>
-    <t>Ashton Jeanty’s early ZAP score is 99.2. If it remains above 99, he’ll join a small group of running backs to achieve that score.    
-He is described as being as good as it gets, with the size to handle a large workload. His best season in prorated reception share is sixth-best in the ZAP model’s history, and his Breakout Score is 94.3.    
-He is one of six players in the model’s database to have a best season total yards per team play above 2.8. There is a possibility that Boise State’s strength of schedule inflated Jeanty’s numbers, but that will be reflected in his draft capital.    
-Finding statistical comparisons for Jeanty is difficult, as there hasn’t been a prospect like him since 2011.    
-Sources and related content</t>
   </si>
   <si>
     <t>Omarion Hampton is a running back from North Carolina. His Breakout Score of 61.7 is slightly below average in this running back class. His top-season reception share is 17.9%, which is third-best in the class. He had a prorated total yards per team play rate last season of 2.48. That was also top-3 among combine invites. He weighs 221 pounds and ran a 4.46 40-yard dash</t>
@@ -464,6 +457,69 @@
   </si>
   <si>
     <t>Tee Higgins, Courtland Sutton, Mike Williams</t>
+  </si>
+  <si>
+    <t>Dylan Sampson has a smaller frame and a less impressive production profile.
+Concerns:
+Smaller size for a running back
+Below-average receiving numbers
+Low Breakout Score
+Below-average in yards after contact and tackle avoidance
+Positive:
+Demonstrates explosiveness
+Overall, there are concerns about his workload and draft capital.</t>
+  </si>
+  <si>
+    <t>Devin Neal has a mixed profile. His 40-yard dash time was underwhelming, but he has a strong production profile with good receiving numbers.
+Strengths:
+Strong production profile.
+Good receiving numbers.
+Effective pass protector.
+Weaknesses:
+Mediocre 40-yard dash time.
+Lack of explosive runs.
+Overall: Neal is a solid prospect, but concerns about his lack of top-end speed limit his potential.
+Projection: Likely to be a worthwhile handcuff rather than a full-blown starter.
+Comparison: Similar to Shane Vereen.</t>
+  </si>
+  <si>
+    <t>Ollie Gordon is a large running back with high volume potential.
+Strengths:
+Size
+Downhill runner
+Capable of handling a large workload
+Weaknesses:
+Lacks top-end speed
+Below-average explosive play rate
+Overall: Gordon's lack of speed limits his upside.
+Projection: His success depends on finding a team that will give him a high volume of carries.
+Comparisons: James Conner and Rhamondre Stevenson</t>
+  </si>
+  <si>
+    <t>Raheim "Rocket" Sanders is a big, fast running back with good age-adjusted receiving production.Strengths:Size and speed combinationGood receiving productionHigh Breakout ScoreWeaknesses:Average explosivenessAverage tackle avoidanceOverall: Sanders has strong ZAP Model metrics.Concerns:His ultimate draft capital is a key factor in evaluating his potential.</t>
+  </si>
+  <si>
+    <t>Ashton Jeanty’s early ZAP score is 99.2. If it remains above 99, he’ll join a small group of running backs to achieve that score.    
+He is described as being as good as it gets, with the size to handle a large workload. His best season in prorated reception share is sixth-best in the ZAP model’s history, and his Breakout Score is 94.3.    
+He is one of six players in the model’s database to have a best season total yards per team play above 2.8. There is a possibility that Boise State’s strength of schedule inflated Jeanty’s numbers, but that will be reflected in his draft capital.    
+Finding statistical comparisons for Jeanty is difficult, as there hasn’t been a prospect like him since 2011.    
+Sources and related content</t>
+  </si>
+  <si>
+    <t>Cam Skattebo has a strong production profile, with high rankings in reception share, Breakout Score, missed tackles forced per attempt, and yards after contact per attempt. However, he has some drawbacks:
+Negatives: He will be 23 years old at the time of the NFL Draft. He lacks top-end speed.
+He has a low career explosive run rate.
+Overall, Skattebo is a difficult prospect to evaluate. His production metrics are promising, but his lack of speed and older age raise concerns about his upside in the NFL.</t>
+  </si>
+  <si>
+    <t>Bhayshul Tuten is a running back who improved his draft stock at the NFL Combine with a fast 40-yard dash and a high Speed Score. He had strong production numbers at both North Carolina A&amp;T and Virginia Tech.
+Strengths: Speed, Production
+Comparisons: Similar to Kenneth Walker (size, speed, Breakout Score). Also compared to Darrynton Evans
+Draft Capital: His draft position will be a key indicator of his potential.
+If drafted in Day 2, it suggests a high likelihood of NFL success.</t>
+  </si>
+  <si>
+    <t>DJ Giddens is an athletic running back with a strong profile.Strengths:Good 40-yard dash time.Impressive vertical and broad jumps.Solid production profile at Kansas State, including receiving ability.Stats:Speed Score over 110.Breakout Score over 75.High yards per team play rate.Comparison:Shares statistical traits with successful NFL running backs like Todd Gurley, Ezekiel Elliott, and others.Giddens' profile suggests he has high potential, and his draft stock should be monitored.</t>
   </si>
 </sst>
 </file>
@@ -845,11 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -899,7 +954,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="232" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -931,10 +986,10 @@
         <v>211</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -966,7 +1021,7 @@
         <v>221</v>
       </c>
       <c r="K3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
@@ -992,7 +1047,7 @@
         <v>62</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>71</v>
@@ -1036,10 +1091,10 @@
         <v>206</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="348" hidden="1" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="348" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1071,7 +1126,7 @@
         <v>202</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="174" x14ac:dyDescent="0.35">
@@ -1106,10 +1161,10 @@
         <v>202</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="203" hidden="1" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="203" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1141,10 +1196,10 @@
         <v>224</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="203" hidden="1" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="203" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1176,7 +1231,7 @@
         <v>221</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
@@ -1211,10 +1266,10 @@
         <v>191</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1263,7 +1318,7 @@
         <v>188</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
@@ -1298,10 +1353,10 @@
         <v>205</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1318,7 +1373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="116" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1348,6 +1403,9 @@
       </c>
       <c r="J15" s="2">
         <v>219</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
@@ -1414,7 +1472,7 @@
         <v>180</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1449,7 +1507,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1480,8 +1538,11 @@
       <c r="J19" s="2">
         <v>206</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K19" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1530,7 +1591,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1561,8 +1622,11 @@
       <c r="J22" s="2">
         <v>212</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K22" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1611,7 +1675,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1628,7 +1692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1658,6 +1722,9 @@
       </c>
       <c r="J26" s="2">
         <v>200</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
@@ -1692,7 +1759,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1722,6 +1789,9 @@
       </c>
       <c r="J28" s="2">
         <v>213</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1788,7 +1858,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="319" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1819,8 +1889,11 @@
       <c r="J31" s="2">
         <v>226</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K31" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1837,7 +1910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1854,7 +1927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1885,8 +1958,11 @@
       <c r="J34" s="2">
         <v>217</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K34" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1918,7 +1994,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1950,7 +2026,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1967,7 +2043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1999,7 +2075,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2031,7 +2107,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2063,7 +2139,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2095,7 +2171,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2127,7 +2203,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2159,7 +2235,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2191,7 +2267,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2223,7 +2299,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2240,7 +2316,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2272,7 +2348,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2337,13 +2413,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K49" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="WR"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K49" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adds formatting for value
</commit_message>
<xml_diff>
--- a/data/1QB_Predraft_Rookies.xlsx
+++ b/data/1QB_Predraft_Rookies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14A95A00-27A9-4084-82D9-D804C18F09F6}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2684AB83-A102-418D-89B0-83329CBF86DF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="38020" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="154">
   <si>
     <t>Rk</t>
   </si>
@@ -459,43 +459,6 @@
     <t>Tee Higgins, Courtland Sutton, Mike Williams</t>
   </si>
   <si>
-    <t>Dylan Sampson has a smaller frame and a less impressive production profile.
-Concerns:
-Smaller size for a running back
-Below-average receiving numbers
-Low Breakout Score
-Below-average in yards after contact and tackle avoidance
-Positive:
-Demonstrates explosiveness
-Overall, there are concerns about his workload and draft capital.</t>
-  </si>
-  <si>
-    <t>Devin Neal has a mixed profile. His 40-yard dash time was underwhelming, but he has a strong production profile with good receiving numbers.
-Strengths:
-Strong production profile.
-Good receiving numbers.
-Effective pass protector.
-Weaknesses:
-Mediocre 40-yard dash time.
-Lack of explosive runs.
-Overall: Neal is a solid prospect, but concerns about his lack of top-end speed limit his potential.
-Projection: Likely to be a worthwhile handcuff rather than a full-blown starter.
-Comparison: Similar to Shane Vereen.</t>
-  </si>
-  <si>
-    <t>Ollie Gordon is a large running back with high volume potential.
-Strengths:
-Size
-Downhill runner
-Capable of handling a large workload
-Weaknesses:
-Lacks top-end speed
-Below-average explosive play rate
-Overall: Gordon's lack of speed limits his upside.
-Projection: His success depends on finding a team that will give him a high volume of carries.
-Comparisons: James Conner and Rhamondre Stevenson</t>
-  </si>
-  <si>
     <t>Raheim "Rocket" Sanders is a big, fast running back with good age-adjusted receiving production.Strengths:Size and speed combinationGood receiving productionHigh Breakout ScoreWeaknesses:Average explosivenessAverage tackle avoidanceOverall: Sanders has strong ZAP Model metrics.Concerns:His ultimate draft capital is a key factor in evaluating his potential.</t>
   </si>
   <si>
@@ -520,6 +483,206 @@
   </si>
   <si>
     <t>DJ Giddens is an athletic running back with a strong profile.Strengths:Good 40-yard dash time.Impressive vertical and broad jumps.Solid production profile at Kansas State, including receiving ability.Stats:Speed Score over 110.Breakout Score over 75.High yards per team play rate.Comparison:Shares statistical traits with successful NFL running backs like Todd Gurley, Ezekiel Elliott, and others.Giddens' profile suggests he has high potential, and his draft stock should be monitored.</t>
+  </si>
+  <si>
+    <t>Elic Ayomanor, a Canadian-born wide receiver with a unique high school path in the US, is entering the NFL draft after only two college seasons at Stanford. Despite a strong sophomore year with over 1,000 yards and a solid Breakout Score, his 2024 performance didn't significantly elevate his stats. He's a prototypical "X" receiver with a large frame and impressive 4.44 40-yard dash time, excelling in downfield targets. While his college numbers are good, not exceptional, his physical attributes and the demand for his position could lead to decent draft capital.</t>
+  </si>
+  <si>
+    <t>The trend in football is shifting towards smaller, lighter wide receivers, but bigger players like Jayden Higgins stand out. At 6’4’’ and 214 pounds, Higgins combines size and smooth athleticism, which is rare for bigger receivers. He's versatile, playing from the slot and all over the formation.
+Higgins' stats improved at Iowa State after transferring from Eastern Kentucky, showing solid production. His Breakout Score of 74.7 and strong yards per route run highlight his potential. Historically, players with similar profiles have had decent success in the NFL. Higgins’ blend of size, versatility, and performance makes him an intriguing prospect.</t>
+  </si>
+  <si>
+    <t>Jaylin Noel, a versatile wide receiver from Iowa State, boasts above-average college stats, ranking in the 60-70th percentile among combine invitees. Primarily a slot receiver, he excelled in short-area targets and screens, evidenced by a low average depth of target (aDOT) early in his career. Despite this, he also demonstrated downfield capability, even surpassing his teammate Jayden Higgins in 20+ yard targets. Noel's versatility extends to special teams, where he returned kicks and punts. His strong combine performance has boosted his draft stock, with some models projecting him higher than others.</t>
+  </si>
+  <si>
+    <t>Jack Bech's NFL draft profile is intertwined with a recent personal tragedy: the loss of his brother, Tiger, in a New Orleans shooting. Bech honored his brother at the Senior Bowl, where he won MVP after scoring the game-winning touchdown. As a prospect, Bech had a promising freshman year at LSU, showing potential alongside future stars Brian Thomas Jr. and Malik Nabers. However, his role was primarily in the slot with short-range targets. After a quiet sophomore year, he transferred to TCU. His senior year was his most productive, but his overall analytical profile, including a below-average Breakout Score, is not particularly strong. Despite this, Bech's versatility, transitioning from a tight end/slot receiver to an "X" receiver, and his production against stiff competition at LSU, are noteworthy. While he has a favorable comparison to Michael Thomas, his overall draft projection is modest.</t>
+  </si>
+  <si>
+    <t>Savion Williams, a physically imposing 6'4", 220+ pound wide receiver from TCU, presents a unique profile due to his dual-threat ability as both a receiver and rusher. While his receiving production was notably low, with the worst adjusted receiving yards per team pass attempt rate in his draft class and a zero Breakout Score, his rushing stats are eye-catching. He recorded 51 carries for 322 yards and 6 touchdowns in his final college season. The ZAP Model values his versatility, particularly his rushing contribution, which boosts his overall evaluation. However, the model also acknowledges the significant risk associated with his poor receiving profile. Historically, wide receivers drafted in the top 100 without a Breakout Score have generally underperformed, with Terry McLaurin being a notable exception. Despite the analytical concerns, Williams's unique skill set could make him an intriguing Day 2 draft pick, offering a high ceiling if he lands in the right offensive system.</t>
+  </si>
+  <si>
+    <t>Jalen Royals, after a brief stint at Georgia Military College, transferred to Utah State, where he had a slow start before a breakout junior season with 71 catches, 1,080 yards, and 15 touchdowns. His senior year further improved his receiving yards per team pass attempt. However, his overall Breakout Score of 43.9 is considered average, reflecting the level of competition at Utah State.
+Projected as a Day 2 draft pick, Royals faces historical challenges, as Day 2 receivers with Breakout Scores below 50 have a lower success rate in producing high fantasy points. Despite this, he possesses athleticism (4.42 40-yard dash) and versatility, playing across the field. The ZAP Model compares him to Rashee Rice, though it acknowledges differences in their college usage and yards-after-catch statistics.</t>
+  </si>
+  <si>
+    <t>Xavier Restrepo, a slot receiver from Miami, lined up in the slot over 90% of his college routes, a high rate that's rare for top-100 draft picks. Historically, receivers with such high slot rates haven't found much NFL success, but the sample size is small.
+Restrepo's production was limited until his final two seasons, where he achieved adjusted receiving yards per team pass attempt rates around 2.40, resulting in a Breakout Score of 48.9. While film analysts praise his route-running and spatial awareness, his production profile is less impressive compared to successful NFL slot receivers like Josh Downs, Christian Kirk, and Cooper Kupp, who had significantly higher Breakout Scores.
+While Restrepo might find a role in the NFL, especially if he receives the projected draft capital, his ceiling as a fantasy football game-changer is questionable based on his college production.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tory Horton looked pretty good through four years of college ball, and then he played in 
+2024, his fifth campaign. He suffered a season-ending knee injury in October, totally 
+derailing the season. Because he played that extra year and didn’t get any production out 
+of it, the ZAP Model only saw that last season as an L. It did nothing but hurt his score.
+ Back in 2020, Horton was at Nevada. He gave us a little production during his two years 
+there, but he really started to cook when he transferred to Colorado State in 2022. That 
+year -- his first season after transferring -- saw him reach a 3.51 prorated receiving 
+yards per team pass attempt rate. That helped produce a Breakout Score of 70.4, the 11th
+best mark in the class. Only three wide receiver combine invites had a season with as 
+strong of a receiving yards per team pass attempt mark, too.
+ Horton had a yards per route run against man that ranked 22nd in college football during 
+his high-end 2022 season, and he can line up all over the field. He doesn’t have a thick 
+build, but there’s good length. He can definitely play a role in the NFL.
+ The question is, will he be good to go coming off of a season-ending injury? Well, this 
+is where the NFL Combine can be helpful. Horton participated in the event, and he ran an 
+impressive 4.41 40. He also did that at 196 pounds, when his listed weight in college was 
+over 10 pounds below that.
+ To me, that subjectively makes Horton even more impressive. He’s definitely a player to 
+watch</t>
+  </si>
+  <si>
+    <t>Ricky White boasts impressive raw production numbers, including high yards per route run and receiving yards per team pass attempt. However, these stats are inflated by the context of his competition at UNLV, in the Mountain West Conference.
+After transferring from Michigan State, where he played behind NFL-caliber receivers, White excelled at UNLV. While his raw numbers are strong, the ZAP Model's adjustments for age and opponent strength result in a Breakout Score of 45.2. This creates a rare profile: a player with high raw production but a low adjusted score.
+Historically, players with this profile have had mixed results, with John Brown being a notable success and Christian Watson still developing. This suggests that White's potential is uncertain.
+As a fantasy analyst, the takeaway is to monitor White's draft capital and landing spot closely. While his raw numbers are enticing, the adjusted metrics suggest caution. He's a player with high potential but also significant risk, and his fantasy value will depend heavily on his NFL opportunity. Avoid overpaying for him based on his raw college stats alone.</t>
+  </si>
+  <si>
+    <t>Tez Johnson, at 154 pounds, is one of the lightest wide receiver prospects in recent NFL draft history. While smaller receivers have found success in the NFL, Johnson's size, combined with a potentially poor combine performance, raises concerns about his draft capital and fantasy potential. Historically, only a few sub-170-pound receivers have achieved significant fantasy production, and those players generally had stronger production profiles and better draft capital than Johnson.
+Johnson's college career spanned five years, with his most productive seasons at Oregon, where he posted impressive yards per route run numbers. However, his receiving yards per team pass attempt were more moderate.
+While Johnson's yards per route run is a positive indicator, similar to recent successes like Ladd McConkey and Puka Nacua, his lack of experience playing outside the slot limits his versatility compared to other successful small receivers.
+As a fantasy analyst, Johnson's size and limited perimeter experience suggest a lower ceiling. While he might find a role in the NFL, the odds of him becoming a high-end fantasy asset are lower than those of other small, but more versatile, receivers. Monitor his draft capital closely, but temper expectations.</t>
+  </si>
+  <si>
+    <t>Tai Felton, despite his low BMI, excels at forcing missed tackles and generating yards after the catch, ranking highly in both categories. However, his overall production profile is average, with a top-season receiving yards per team pass attempt of 2.28 and a Breakout Score of 56.3.
+Concerns exist about his play strength translating to the NFL, and his statistical comparisons are to players with similar builds who have struggled. His 4.37 speed is a potential asset, but relying solely on speed for NFL success is risky.
+Overall, Felton's profile is unremarkable, leading the ZAP Model to project him as a benchwarmer. As a fantasy analyst, he presents a low-ceiling prospect with limited upside.</t>
+  </si>
+  <si>
+    <t>Nick Nash, a former quarterback turned wide receiver, had a remarkable 2024 season at San Jose State, winning the college football "triple crown" in receptions, receiving yards, and receiving touchdowns. 1  However, his raw production needs context.   
+Despite his impressive raw numbers, his adjusted metrics, such as receiving yards per team pass attempt (2.71) and yards per route run (2.71), are merely average compared to other combine invitees. His age (almost 25) and the level of competition in the Mountain West Conference further temper his evaluation. His transition from quarterback to wide receiver is unique, but his Breakout Score of zero reflects the challenges posed by his age and program strength. While his 2024 season was undeniably productive, especially against larger programs, the raw numbers don't paint the full picture. As a fantasy analyst, Nash's size and recent success are intriguing, but his advanced age and adjusted metrics suggest caution. He's a developmental prospect with a potentially limited ceiling, and his raw stats should be viewed with skepticism.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pat Bryant’s stat lines across his four years at Illinois show pretty good yearly 
+progression. He only had 98 yards as a Freshman, then it was 453 as a Sophomore, 560 as a 
+Junior, and 984 as a Senior.
+ But that Senior year -- 2024 -- looks much better in the ZAP Model than you might think. 
+His prorated receiving yards per team pass attempt last year was 3.02, and, given the 
+teams Illinois faced, his adjusted number looks even better. That’s more than double his 
+receiving yards per team pass attempt mark from any other collegiate season.
+ A Senior-year breakout isn’t something we’re desperately searching for, but we’re not 
+talking about some high-end, obvious prospect who’s going to cost a lot during your rookie 
+draft. Bryant came through with a solid 72.4 Breakout Score, something achieved by just 10 
+wide receivers in this year’s class.
+ From 2011 to 2022 –- this allows us to analyze wideouts in the ZAP Model database who’ve 
+played three years in the NFL -- we’ve had 22 wide receivers hit a best-season yards per 
+team pass attempt of 2.75 (Bryant was at 3.02) and a Breakout Score of 60 (Bryant was at 
+72.4) while getting drafted after Pick 120. Of those 22 wideouts, 4 were able to score 
+double-digit PPR points per game across their first three years in the league. That’s a 
+rate of 18%.
+ When looking at the group opposite of that, the 10-plus PPR points per game rate falls to 
+4.9%. 
+Late-round wide receivers don’t provide much fantasy relevancy. We get hits and remember 
+when we do, but they’re rare. With Bryant, we’re at least looking at some marks that 
+typically hit. Add on the fact that he’s a lengthy wide receiver who can play all over the 
+formation, and you’ve got yourself a possible sleeper.</t>
+  </si>
+  <si>
+    <t>Dylan Sampson, while possessing a 200-pound frame, doesn't align with the ideal size profile for high-end fantasy running backs. His production profile also doesn't compensate for this.
+Across his three seasons at Tennessee, Sampson's rushing volume increased, but his receiving numbers remained underwhelming, culminating in a best-season reception share of only 8.5% and a below-average Breakout Score of 45.0.
+His total yards per team play and yards after contact per attempt are also below average, and his tackle avoidance is considered ordinary. While he displayed some explosive runs, his absence at the combine leaves his speed untested.
+Sampson's potential NFL workload is a concern. Historically, coaches tend to limit the usage of 200-pound backs, and his limited receiving ability further diminishes his fantasy prospects. Consequently, he risks a negative Draft Capital Delta.</t>
+  </si>
+  <si>
+    <t>Devin Neal's 4.58 40-yard dash time at the combine was underwhelming, failing to enhance his otherwise strong production profile. However, his overall ZAP Model score remains solid.
+Neal demonstrated consistent production across his four seasons at Kansas, including consecutive 1,200-yard rushing campaigns. Notably, his receiving numbers were excellent, placing him among the top five running backs in this class with a best-season reception share of at least 13% and a Breakout Score above 85.
+While his explosive run rate is below average, his pass protection skills, as graded by PFF, are a significant asset. This could facilitate early NFL playing time.
+Despite his solid overall profile, the primary concern is a lack of explosive running ability, potentially limiting him to a handcuff role rather than a starting position. His success hinges on a team utilizing his pass protection and receiving abilities, similar to his top comparable, Shane Vereen.</t>
+  </si>
+  <si>
+    <t>Ollie Gordon's 4.61 40-yard dash was mitigated by his significant 226-pound frame, resulting in a respectable Speed Score. He had a stellar 2023 season at Oklahoma State, leading the nation in rushing yards and winning the Doak Walker Award. 1  However, his production dipped in 2024.   
+Gordon's size and downhill running style suggest he can handle a substantial workload. However, his lack of elite speed and below-average explosive play rate limit his upside, making volume crucial for fantasy success.
+While players like James Conner and Rhamondre Stevenson have thrived with similar profiles, the depth of this running back class could lead to Gordon being part of a committee, limiting his immediate fantasy impact.
+He has the potential for high volume in the right situation, but it's uncertain if he'll command a significant workload early in his NFL career.</t>
+  </si>
+  <si>
+    <t>Trevor Etienne is projected to have a "Low Risk" Draft Capital Delta due to his strong ZAP Model evaluation, primarily driven by his pass-catching abilities.
+Despite his undersized 198-pound frame and limited collegiate workload (never exceeding 133 carries in a season), Etienne excels as a receiver. His top-season reception share ranks 10th in his class, and his Breakout Score is 11th.
+However, his yards per team play rate never exceeded 1.25, reflecting his limited rushing volume. Notably, his best-season yards per team play is among the lowest in his class.
+Despite this, historically, running backs with similar profiles—high Breakout Scores but low yards per team play—have found success as receivers in the NFL. Examples include Josh Jacobs, Tony Pollard, and James Cook.
+Etienne's NFL role is likely as a pass-catching back, not a high-volume rusher. He's dynamic with the ball and projects as valuable PPR depth, even if he doesn't reach his brother's fantasy heights.</t>
+  </si>
+  <si>
+    <t>Brashard Smith's unique journey from wide receiver at Miami to running back at SMU makes him an intriguing prospect.
+* **Transition and Production:** He excelled in his single season as a running back, rushing for 1,332 yards and showcasing explosive speed with a sub-4.4 40-yard dash.
+* **Comparison to Tyrone Tracy:** While similar in position change, Smith is smaller (194 pounds) than Tracy (209 pounds) and has less running back experience.
+* **Size Concerns:** Historically, smaller running backs (under 200 pounds) rarely command high rushing workloads in the NFL.
+* **Projected Role:** Smith is likely to begin his NFL career as a situational or mismatch player, leveraging his speed and agility.
+* **Fantasy Outlook:** He's projected as a bench stash, with potential for more if he develops, but his size limits his likely early career volume.</t>
+  </si>
+  <si>
+    <t>RJ Harvey presents an intriguing profile with a compact build similar to Jaylen Warren, but with a stronger production profile.
+Strong Production: He boasts a solid 11.1% top-year reception share and an impressive 2.23 max-season total yards per team play rate, ranking highly in his class.
+Combine Performance: His 4.40 40-yard dash resulted in a 109.4 Speed Score, highlighting his athleticism.1   
+Age Concerns: At 24, Harvey's age is a significant factor. He began as a quarterback at Virginia in 2019, transferred to UCF, and faced setbacks including the pandemic and an ACL tear.
+Historical Context: Historically, 24-year-old running back prospects have not yielded consistent, long-term fantasy success. Ray Davis and Tyrone Tracy are recent examples, but their NFL outcomes are yet to be determined.
+Fantasy Outlook: Harvey's production and athleticism are appealing, but his age introduces risk. He could be a valuable contributor, but his long-term fantasy potential is uncertain</t>
+  </si>
+  <si>
+    <t>LeQuint Allen boasts an exceptional receiving profile, ranking near the top of his class in reception share and Breakout Score. However, his rushing metrics are concerning.
+Receiving Dominance: He possesses elite receiving numbers, with a high reception share and Breakout Score, indicating significant pass-catching potential.
+Rushing Concerns: His tackle avoidance and yards after contact per attempt are below average, raising questions about his effectiveness as a rusher.
+Draft Capital Impact: His receiving profile is highly valuable, but it's heavily dependent on draft capital. A Day 3 selection would significantly diminish his fantasy prospects.
+Historical Precedent: Historically, running backs with similar receiving profiles but lower draft capital have had limited success, with Kyren Williams being a notable exception.
+Combine Uncertainty: Allen's decision to skip the combine leaves his speed and athleticism unknown, adding to the uncertainty surrounding his projection.
+Fantasy Outlook: Despite the rushing concerns, Allen's pass-catching prowess makes him an intriguing PPR prospect, especially given his young age. His fantasy value is heavily tied to his draft position.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jarquez Hunter has the third-best Breakout Score in this year’s draft class. It seems wild 
+because he topped out at a 10.7% reception share at Auburn, which isn’t anything special. 
+His Breakout Score is high, though, because, as a Sophomore, Hunter had 224 receiving yards 
+on a team that threw it just 308 times. He was efficient with his touches.
+ The combination of high-end Breakout Score and slightly-above-average reception share 
+isn’t common. In fact, there’s only been one other running back in ZAP Model history with 
+a Breakout Score above 90 (Hunter is at 93.8) and a best-season reception share below 11% 
+(Hunter is at 10.7%). 
+The other guy to do it? Kenneth Walker.
+ Hunter didn’t have quite the same rushing performance as Walker in college, but don’t 
+mistake that for him being a poor runner. Compared to the rest of the class, Hunter was 
+fifth in career avoided tackles per rush, ninth in career explosive run rate, and ninth in 
+career yards after contact per attempt. Shoutout to PFF for that data.
+ Within a class littered with talent, Hunter stands out as a strong sleeper in the later 
+rounds. He can do it all, and he showed at the NFL Combine that his speed is underrated, 
+too, after running a 4.44 in the 40. Keep an eye on him throughout the draft process.</t>
+  </si>
+  <si>
+    <t>We have a ton of great pass-catchers in this year’s draft class. So many of our 31 NFL 
+Combine invites came with strong receiving numbers in the ZAP Model.
+ Damien Martinez’s profile is lacking a bit there. His top year in prorated reception share 
+is just 5.4%, second-worst in the class. He did have a 41.1 Breakout Score, but that’s not 
+exactly what we’re looking for here.
+ From 2011 to 2022, we’ve seen 44 running backs get drafted with best-season reception 
+shares below 7%. Of those 44, only two scored more than 13 PPR points per game in one of 
+their first three seasons.
+ This isn’t everything for Martinez. After all, the backs who do succeed with his type 
+of receiving numbers tend to be bigger in size, and Martinez was nearly 220 pounds at 
+this year’s combine. He also ran a 4.51, giving him a 104.9 Speed Score, well above the 
+threshold we’re looking for these guys to get to.
+ We just probably won’t see Martinez deployed much as a receiver in the NFL. Going back to 
+those 44 running backs with sub-7% best-season reception shares, only two of them were able 
+to get to a double-digit percentage target share in one of their first three NFL seasons. 
+And neither player was able to do it more than once. The vast majority of them were under 
+the 5% target share mark as pros.
+ Martinez is an angry runner who can lock up early-down work, but, especially in PPR 
+formats, we’ll need more pass-catching for a true ceiling to be hit</t>
+  </si>
+  <si>
+    <t>Montrell Johnson was faster than anticipated at the NFL Combine, running a 4.41 40-yard 
+dash. At 212 pounds, that gave him the second-best Speed Score in the class, behind only 
+Bhayshul Tuten. 
+Should we care? I mean, kind of? It’s always nice when there’s a specific trait we can 
+target with a late-round dart throw, and Speed Scores that high don’t grow on trees.
+ Johnson’s performance at the combine was necessary for the ZAP Model, too, because there’s 
+not a whole lot going for him outisde of it. His top season in total yards per team play 
+was just 1.30 across his four years of college, fourth-worst in the class. When looking at 
+the ZAP Model’s history, there’ve been just nine backs who scored 14 or more PPR points per 
+game in either Year 1, Year 2, or Year 3 in the NFL who had a max-season total yards per 
+team play rate below 1.40. Only four of them were drafted past Pick 100.
+ One of those players is Isiah Pacheco, who’s Johnson’s top comp. Pacheco runs with more 
+ferosity than almost any running back in the league, and that’s allowed him to find some 
+success, but the two backs are similar in size, have elite Speed Scores, and both struggled 
+a bit on the production front.
+ Johnson could be a solid early-down runner with some upside on the right team in the NFL. 
+We don’t get to say this a lot, but his combine performance saved him analytically</t>
   </si>
 </sst>
 </file>
@@ -904,7 +1067,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -986,7 +1149,7 @@
         <v>211</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1405,10 +1568,10 @@
         <v>219</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1438,6 +1601,9 @@
       </c>
       <c r="J16" s="2">
         <v>206</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
@@ -1475,7 +1641,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1505,6 +1671,9 @@
       </c>
       <c r="J18" s="2">
         <v>214</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
@@ -1539,7 +1708,7 @@
         <v>206</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -1559,7 +1728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="116" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1589,6 +1758,9 @@
       </c>
       <c r="J21" s="2">
         <v>194</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -1623,7 +1795,7 @@
         <v>212</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -1643,7 +1815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1673,6 +1845,9 @@
       </c>
       <c r="J24" s="2">
         <v>205</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -1692,7 +1867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1724,10 +1899,10 @@
         <v>200</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1758,8 +1933,11 @@
       <c r="J27" s="2">
         <v>214</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="K27" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="232" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1791,10 +1969,10 @@
         <v>213</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1825,8 +2003,11 @@
       <c r="J29" s="2">
         <v>196</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="K29" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="203" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1857,8 +2038,11 @@
       <c r="J30" s="2">
         <v>209</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="319" x14ac:dyDescent="0.35">
+      <c r="K30" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1890,7 +2074,7 @@
         <v>226</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -1959,10 +2143,10 @@
         <v>217</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1993,8 +2177,11 @@
       <c r="J35" s="2">
         <v>205</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="K35" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="348" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2024,6 +2211,9 @@
       </c>
       <c r="J36" s="2">
         <v>204</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -2043,7 +2233,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="261" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2074,8 +2264,11 @@
       <c r="J38" s="2">
         <v>198</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="K38" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="261" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2106,8 +2299,11 @@
       <c r="J39" s="2">
         <v>184</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="K39" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="174" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2138,8 +2334,11 @@
       <c r="J40" s="2">
         <v>222</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="K40" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2170,8 +2369,11 @@
       <c r="J41" s="2">
         <v>204</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="K41" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="232" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2202,8 +2404,11 @@
       <c r="J42" s="2">
         <v>154</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="K42" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2234,8 +2439,11 @@
       <c r="J43" s="2">
         <v>194</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="K43" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="377" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2266,8 +2474,11 @@
       <c r="J44" s="2">
         <v>217</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="K44" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="174" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2297,6 +2508,9 @@
       </c>
       <c r="J45" s="2">
         <v>183</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
@@ -2316,7 +2530,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2347,8 +2561,11 @@
       <c r="J47" s="2">
         <v>212</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="K47" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2379,8 +2596,11 @@
       <c r="J48" s="2">
         <v>204</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="K48" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="203" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2410,6 +2630,9 @@
       </c>
       <c r="J49" s="2">
         <v>203</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds RSP and conditional formatting
</commit_message>
<xml_diff>
--- a/data/1QB_Predraft_Rookies.xlsx
+++ b/data/1QB_Predraft_Rookies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2684AB83-A102-418D-89B0-83329CBF86DF}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE92ECD4-50FB-4FBF-8078-E7B983B4AE84}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="38020" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="157">
   <si>
     <t>Rk</t>
   </si>
@@ -683,6 +683,37 @@
 a bit on the production front.
  Johnson could be a solid early-down runner with some upside on the right team in the NFL. 
 We don’t get to say this a lot, but his combine performance saved him analytically</t>
+  </si>
+  <si>
+    <t>Tahj Brooks</t>
+  </si>
+  <si>
+    <t>Trayveon Williams, Ray Davis, Jeremy McNichols</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tahj Brooks is built to see a lot of work. He was only 5’9’’ at the combine, but he weighed 
+in at 214 pounds, giving him a top-three Body Mass Index in this year’s class.
+ Brooks spent five seasons at Texas Tech, and he was really featured in the offense during 
+his final two. In 2023 and 2024, Brooks saw 290 and 284 rush attempts, respectively, and he 
+hit total yards per team play rates of 1.71 and 1.99. That 1.99 number ranks top-10 in the 
+class.
+ There may be some long speed concerns with Brooks, even if he exceeded expectations a bit 
+at the combine with a 4.52 40. He was below average at generating explosive runs throughout 
+his career. His receiving profile isn’t stellar, either, with a bottom-10 best-season 
+receiving yards per team pass attempt rate. Brooks’ 35.7 Breakout Score is seventh-worst in 
+the class.
+ We’ve had successes in the ZAP Model database from backs who had sub-40 Breakout Scores, 
+but those wins haven’t typically been long-term ones. Here’s a list of backs with a 
+Breakout Score below 40 to have given fantasy managers 14 or more PPR points per game in 
+one of their first three seasons in the league: Alfred Morris, Andre Ellington, Carlos 
+Hyde, Melvin Gordon, Jordan Howard, Chris Carson, Miles Sanders, and James Robinson. There 
+are a lot of one-hit wonders in there. The best back in the group, Melvin Gordon, at least 
+had draft capital backing him, too.
+ That same filter -- backs with Breakout Scores below 40 -- also hasn’t provided a lot of 
+receiving upside. Just nine backs in the model with that low of a Breakout Score ended up 
+reaching a 10% target share per game rate in one of their first three seasons. 
+Brooks can handle a lot of work -- he’s not a bad prospect -- but I’m not sure he’ll get 
+the opportunity to be a true three-down back in the NFL. </t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2635,6 +2666,41 @@
         <v>142</v>
       </c>
     </row>
+    <row r="50" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <v>20</v>
+      </c>
+      <c r="E50">
+        <v>14</v>
+      </c>
+      <c r="F50">
+        <v>46</v>
+      </c>
+      <c r="G50" t="s">
+        <v>83</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J50" s="2">
+        <v>214</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K49" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adds Buttons for more functionality and removes quotes from analysis
</commit_message>
<xml_diff>
--- a/data/1QB_Predraft_Rookies.xlsx
+++ b/data/1QB_Predraft_Rookies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE92ECD4-50FB-4FBF-8078-E7B983B4AE84}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACF64577-6B27-4FD3-9B9E-364ABD428618}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="38020" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15460" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,12 +383,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Tetairoa McMillan is an early-declare wide receiver with a lot of size, who gave Arizona solid production.   
-His Breakout Score is good, but not amazing, sitting at 83.1. His raw numbers in yards per team attempt were good, but they were brought down a bit when adjusted for the strength of the opponent.   
-His comparisons to Drake London don’t work well analytically, as London had a much better age-adjusted profile. London's Breakout Score was elite. Profiles like Tee Higgins and Courtland Sutton make a lot more sense. They didn’t get the draft capital McMillan is likely to get, but their fantasy impacts have definitely been felt.   
-</t>
-  </si>
-  <si>
     <t>Omarion Hampton is a running back from North Carolina. His Breakout Score of 61.7 is slightly below average in this running back class. His top-season reception share is 17.9%, which is third-best in the class. He had a prorated total yards per team play rate last season of 2.48. That was also top-3 among combine invites. He weighs 221 pounds and ran a 4.46 40-yard dash</t>
   </si>
   <si>
@@ -420,26 +414,6 @@
   <si>
     <t xml:space="preserve">The rushing portion to Quinshon Judkins’ profile is pretty wild.  As a Freshman at Ole Miss, Judkins ran the ball 274 times for 1,567 yards and 16 scores.  And he did that on a team that had an NFLer in Zach Evans.  After another successful Sophomore year, Judkins decided to chase a national championship at Ohio State for his third and final college season.  And he, alongside running back teammate TreVeyon Henderson, got it.  As impressive as Judkins’ production was throughout college, the ZAP Model isn’t as in love.  Because his receiving numbers weren’t as good.  Judkins had a best-season reception share of 8.6%, a number acquired during his second year at Mississippi.  He ran about 100 fewer routes than Henderson last season, though the two of them finished the year with a nearly identical yards per route run rate.  Judkins Breakout Score was below average, too, at just 46.5.  The class average Breakout Score is 59.4.  I don’t think Judkins is incapable of being a decent receiving threat in the NFL, but there’s a chance we see him and his size focused more on early-down stuff.    
 </t>
-  </si>
-  <si>
-    <t>The ZAP Model has seen nearly 60 wide receivers hit 14 or more PPR points per game in one of their first three seasons in the league.  Just 5 of those 60 did it with a best-season receiving yards per team pass attempt rate below 2.0.  One is Tyreek Hill, who we know is an outlier.  Another is Hunter Renfrow, who only gave us one good year.  The other three are Terry McLaurin, Nico Collins, and Ladd McConkey.    
-Matthew Golden’s best prorated receiving yards per team pass attempt figure was below 2.0.  It was 1.82, done in 2024, his third and final year of college football.  When we adjust for program strength, his top year in yards per team pass attempt is 2.28, not 1.82.  Those team strength adjustments are a key reason Golden’s Breakout Score is an OK-enough 51.4.    
-Golden started his college life at Houston, where he played two seasons and gave us some production.  Receiving yard per team pass attempt rates of 1.38 and 1.32 as a Freshman and Sophomore aren’t tragic.  His top season in yards per route run, per PFF, was 2.10.    
-Golden is probably going to get solid draft capital given his ability to create explosive plays.  He's easy to like on film, and his most favorable comparable in the ZAP Model is Ladd McConkey.  So there are things working in his favor.  He’s just not close to a flawless prospect analytically.</t>
-  </si>
-  <si>
-    <t>When the initial NFL Combine list came out, the Heisman-winning Travis Hunter was only listed as a cornerback. That changed as we got closer to the combine, as he was added to the wide receiver list.  No one really knows how Hunter is going to be used at the next level.  Some believe that he'll be a full-time corner who takes some snaps on offense.  If he's a part-time player on offense, then he'll have a hard time living up to his ZAP score.    
-His production profile is kind of ordinary for a first-rounder.  His top year in receiving yards per team pass attempt came last season, where it was 2.61.  That's a 20th percentile number among all first-round wide receivers since 2011.  His Breakout Score of 66.9 is a 15th percentile one compared to other first-rounders.  His career yards per route run looks slightly better, but, among first-round wide receivers over the last five seasons, it's still below average.  His yards per route run rate was 2.51 last season.  There are 27 wide receivers in this year's class who had a better rate than that during one of their collegiate seasons.    
-We can probably cut Hunter a bit of a break because, you know, he was playing on both offense and defense in college.  None of this is to take away from his insane gifts.  And, to be fair, a lot of evaluators who look solely at film think Hunter is as good as it gets.  If there were no restrictions here -- if we were simply assuming he would play wide receiver -- then I'd more than likely be lower than the market on Hunter.  It's very possible that his metrics aren't showing up well because, again, he did everything for Colorado.  But if we're being completely objective, the predictive metrics we look at aren't close to excellent.</t>
-  </si>
-  <si>
-    <t>No wide receiver in this year's draft class has a higher best-season adjusted receiving yards per team pass attempt than Tre Harris.  Harris' final season at Ole Miss was great.  A 60-catch, 1,030-yard campaign may not look like much, but he amassed that in just eight games.  That led to a (prorated) receiving yards per team pass attempt of 3.86.  Harris' yards per route run last year was even crazier.  According to Pro Football Focus, he saw over five yards per route run.  Not only was that by far the highest in this year's class, but it was the highest PFF has ever recorded from a Power Five wideout with 100 or more routes run.  That dates back to 2014.    
-As impressive as that is, it wasn't all butterflies and rainbows throughout Harris' college career.  He started things off at Louisiana Tech, where he played three seasons.  There, he failed to really break out until his third year.  He then went to Ole Miss where he had back-to-back seasons of strong production, including his ridiculous 2024.    
-We're not usually looking for wide receivers who played five years of college ball.  Younger receivers give us better fantasy football odds.  But, because Harris' numbers were so good at Ole Miss, he ended up with a pretty impressive 83.4 Breakout Score, a top-three number in the class.    
-Older players generally don't have upper-tier Breakout Scores in the model.  Since Breakout Score incorporates age, higher scores tend to correlate with at least average-aged prospects.    
-Harris is an exception.  Especially when you layer on projected draft capital.    
-If Harris gets drafted in the top-100 he's currently forecasted to go in Round 2 then he'll become just the third wideout in ZAP Model history to get picked in the top-100 after turning 23 years old with a Breakout Score above 80. [cite: 4358, 4359, 480.9] The other two?  Sterling Shepard, who had a pretty decent career in the league, and Calvin Ridley.  NFL teams are always looking for perimeter players with decent size.  Harris has that.  And he might be pretty good, too.  He's a higher-variance player to watch.    
-Sources and related content</t>
   </si>
   <si>
     <t>Started playing college football at Alabama.
@@ -459,9 +433,6 @@
     <t>Tee Higgins, Courtland Sutton, Mike Williams</t>
   </si>
   <si>
-    <t>Raheim "Rocket" Sanders is a big, fast running back with good age-adjusted receiving production.Strengths:Size and speed combinationGood receiving productionHigh Breakout ScoreWeaknesses:Average explosivenessAverage tackle avoidanceOverall: Sanders has strong ZAP Model metrics.Concerns:His ultimate draft capital is a key factor in evaluating his potential.</t>
-  </si>
-  <si>
     <t>Ashton Jeanty’s early ZAP score is 99.2. If it remains above 99, he’ll join a small group of running backs to achieve that score.    
 He is described as being as good as it gets, with the size to handle a large workload. His best season in prorated reception share is sixth-best in the ZAP model’s history, and his Breakout Score is 94.3.    
 He is one of six players in the model’s database to have a best season total yards per team play above 2.8. There is a possibility that Boise State’s strength of schedule inflated Jeanty’s numbers, but that will be reflected in his draft capital.    
@@ -482,32 +453,8 @@
 If drafted in Day 2, it suggests a high likelihood of NFL success.</t>
   </si>
   <si>
-    <t>DJ Giddens is an athletic running back with a strong profile.Strengths:Good 40-yard dash time.Impressive vertical and broad jumps.Solid production profile at Kansas State, including receiving ability.Stats:Speed Score over 110.Breakout Score over 75.High yards per team play rate.Comparison:Shares statistical traits with successful NFL running backs like Todd Gurley, Ezekiel Elliott, and others.Giddens' profile suggests he has high potential, and his draft stock should be monitored.</t>
-  </si>
-  <si>
-    <t>Elic Ayomanor, a Canadian-born wide receiver with a unique high school path in the US, is entering the NFL draft after only two college seasons at Stanford. Despite a strong sophomore year with over 1,000 yards and a solid Breakout Score, his 2024 performance didn't significantly elevate his stats. He's a prototypical "X" receiver with a large frame and impressive 4.44 40-yard dash time, excelling in downfield targets. While his college numbers are good, not exceptional, his physical attributes and the demand for his position could lead to decent draft capital.</t>
-  </si>
-  <si>
-    <t>The trend in football is shifting towards smaller, lighter wide receivers, but bigger players like Jayden Higgins stand out. At 6’4’’ and 214 pounds, Higgins combines size and smooth athleticism, which is rare for bigger receivers. He's versatile, playing from the slot and all over the formation.
-Higgins' stats improved at Iowa State after transferring from Eastern Kentucky, showing solid production. His Breakout Score of 74.7 and strong yards per route run highlight his potential. Historically, players with similar profiles have had decent success in the NFL. Higgins’ blend of size, versatility, and performance makes him an intriguing prospect.</t>
-  </si>
-  <si>
-    <t>Jaylin Noel, a versatile wide receiver from Iowa State, boasts above-average college stats, ranking in the 60-70th percentile among combine invitees. Primarily a slot receiver, he excelled in short-area targets and screens, evidenced by a low average depth of target (aDOT) early in his career. Despite this, he also demonstrated downfield capability, even surpassing his teammate Jayden Higgins in 20+ yard targets. Noel's versatility extends to special teams, where he returned kicks and punts. His strong combine performance has boosted his draft stock, with some models projecting him higher than others.</t>
-  </si>
-  <si>
-    <t>Jack Bech's NFL draft profile is intertwined with a recent personal tragedy: the loss of his brother, Tiger, in a New Orleans shooting. Bech honored his brother at the Senior Bowl, where he won MVP after scoring the game-winning touchdown. As a prospect, Bech had a promising freshman year at LSU, showing potential alongside future stars Brian Thomas Jr. and Malik Nabers. However, his role was primarily in the slot with short-range targets. After a quiet sophomore year, he transferred to TCU. His senior year was his most productive, but his overall analytical profile, including a below-average Breakout Score, is not particularly strong. Despite this, Bech's versatility, transitioning from a tight end/slot receiver to an "X" receiver, and his production against stiff competition at LSU, are noteworthy. While he has a favorable comparison to Michael Thomas, his overall draft projection is modest.</t>
-  </si>
-  <si>
-    <t>Savion Williams, a physically imposing 6'4", 220+ pound wide receiver from TCU, presents a unique profile due to his dual-threat ability as both a receiver and rusher. While his receiving production was notably low, with the worst adjusted receiving yards per team pass attempt rate in his draft class and a zero Breakout Score, his rushing stats are eye-catching. He recorded 51 carries for 322 yards and 6 touchdowns in his final college season. The ZAP Model values his versatility, particularly his rushing contribution, which boosts his overall evaluation. However, the model also acknowledges the significant risk associated with his poor receiving profile. Historically, wide receivers drafted in the top 100 without a Breakout Score have generally underperformed, with Terry McLaurin being a notable exception. Despite the analytical concerns, Williams's unique skill set could make him an intriguing Day 2 draft pick, offering a high ceiling if he lands in the right offensive system.</t>
-  </si>
-  <si>
     <t>Jalen Royals, after a brief stint at Georgia Military College, transferred to Utah State, where he had a slow start before a breakout junior season with 71 catches, 1,080 yards, and 15 touchdowns. His senior year further improved his receiving yards per team pass attempt. However, his overall Breakout Score of 43.9 is considered average, reflecting the level of competition at Utah State.
 Projected as a Day 2 draft pick, Royals faces historical challenges, as Day 2 receivers with Breakout Scores below 50 have a lower success rate in producing high fantasy points. Despite this, he possesses athleticism (4.42 40-yard dash) and versatility, playing across the field. The ZAP Model compares him to Rashee Rice, though it acknowledges differences in their college usage and yards-after-catch statistics.</t>
-  </si>
-  <si>
-    <t>Xavier Restrepo, a slot receiver from Miami, lined up in the slot over 90% of his college routes, a high rate that's rare for top-100 draft picks. Historically, receivers with such high slot rates haven't found much NFL success, but the sample size is small.
-Restrepo's production was limited until his final two seasons, where he achieved adjusted receiving yards per team pass attempt rates around 2.40, resulting in a Breakout Score of 48.9. While film analysts praise his route-running and spatial awareness, his production profile is less impressive compared to successful NFL slot receivers like Josh Downs, Christian Kirk, and Cooper Kupp, who had significantly higher Breakout Scores.
-While Restrepo might find a role in the NFL, especially if he receives the projected draft capital, his ceiling as a fantasy football game-changer is questionable based on his college production.</t>
   </si>
   <si>
     <t xml:space="preserve"> Tory Horton looked pretty good through four years of college ball, and then he played in 
@@ -529,27 +476,6 @@
 over 10 pounds below that.
  To me, that subjectively makes Horton even more impressive. He’s definitely a player to 
 watch</t>
-  </si>
-  <si>
-    <t>Ricky White boasts impressive raw production numbers, including high yards per route run and receiving yards per team pass attempt. However, these stats are inflated by the context of his competition at UNLV, in the Mountain West Conference.
-After transferring from Michigan State, where he played behind NFL-caliber receivers, White excelled at UNLV. While his raw numbers are strong, the ZAP Model's adjustments for age and opponent strength result in a Breakout Score of 45.2. This creates a rare profile: a player with high raw production but a low adjusted score.
-Historically, players with this profile have had mixed results, with John Brown being a notable success and Christian Watson still developing. This suggests that White's potential is uncertain.
-As a fantasy analyst, the takeaway is to monitor White's draft capital and landing spot closely. While his raw numbers are enticing, the adjusted metrics suggest caution. He's a player with high potential but also significant risk, and his fantasy value will depend heavily on his NFL opportunity. Avoid overpaying for him based on his raw college stats alone.</t>
-  </si>
-  <si>
-    <t>Tez Johnson, at 154 pounds, is one of the lightest wide receiver prospects in recent NFL draft history. While smaller receivers have found success in the NFL, Johnson's size, combined with a potentially poor combine performance, raises concerns about his draft capital and fantasy potential. Historically, only a few sub-170-pound receivers have achieved significant fantasy production, and those players generally had stronger production profiles and better draft capital than Johnson.
-Johnson's college career spanned five years, with his most productive seasons at Oregon, where he posted impressive yards per route run numbers. However, his receiving yards per team pass attempt were more moderate.
-While Johnson's yards per route run is a positive indicator, similar to recent successes like Ladd McConkey and Puka Nacua, his lack of experience playing outside the slot limits his versatility compared to other successful small receivers.
-As a fantasy analyst, Johnson's size and limited perimeter experience suggest a lower ceiling. While he might find a role in the NFL, the odds of him becoming a high-end fantasy asset are lower than those of other small, but more versatile, receivers. Monitor his draft capital closely, but temper expectations.</t>
-  </si>
-  <si>
-    <t>Tai Felton, despite his low BMI, excels at forcing missed tackles and generating yards after the catch, ranking highly in both categories. However, his overall production profile is average, with a top-season receiving yards per team pass attempt of 2.28 and a Breakout Score of 56.3.
-Concerns exist about his play strength translating to the NFL, and his statistical comparisons are to players with similar builds who have struggled. His 4.37 speed is a potential asset, but relying solely on speed for NFL success is risky.
-Overall, Felton's profile is unremarkable, leading the ZAP Model to project him as a benchwarmer. As a fantasy analyst, he presents a low-ceiling prospect with limited upside.</t>
-  </si>
-  <si>
-    <t>Nick Nash, a former quarterback turned wide receiver, had a remarkable 2024 season at San Jose State, winning the college football "triple crown" in receptions, receiving yards, and receiving touchdowns. 1  However, his raw production needs context.   
-Despite his impressive raw numbers, his adjusted metrics, such as receiving yards per team pass attempt (2.71) and yards per route run (2.71), are merely average compared to other combine invitees. His age (almost 25) and the level of competition in the Mountain West Conference further temper his evaluation. His transition from quarterback to wide receiver is unique, but his Breakout Score of zero reflects the challenges posed by his age and program strength. While his 2024 season was undeniably productive, especially against larger programs, the raw numbers don't paint the full picture. As a fantasy analyst, Nash's size and recent success are intriguing, but his advanced age and adjusted metrics suggest caution. He's a developmental prospect with a potentially limited ceiling, and his raw stats should be viewed with skepticism.</t>
   </si>
   <si>
     <t xml:space="preserve"> Pat Bryant’s stat lines across his four years at Illinois show pretty good yearly 
@@ -577,56 +503,6 @@
 formation, and you’ve got yourself a possible sleeper.</t>
   </si>
   <si>
-    <t>Dylan Sampson, while possessing a 200-pound frame, doesn't align with the ideal size profile for high-end fantasy running backs. His production profile also doesn't compensate for this.
-Across his three seasons at Tennessee, Sampson's rushing volume increased, but his receiving numbers remained underwhelming, culminating in a best-season reception share of only 8.5% and a below-average Breakout Score of 45.0.
-His total yards per team play and yards after contact per attempt are also below average, and his tackle avoidance is considered ordinary. While he displayed some explosive runs, his absence at the combine leaves his speed untested.
-Sampson's potential NFL workload is a concern. Historically, coaches tend to limit the usage of 200-pound backs, and his limited receiving ability further diminishes his fantasy prospects. Consequently, he risks a negative Draft Capital Delta.</t>
-  </si>
-  <si>
-    <t>Devin Neal's 4.58 40-yard dash time at the combine was underwhelming, failing to enhance his otherwise strong production profile. However, his overall ZAP Model score remains solid.
-Neal demonstrated consistent production across his four seasons at Kansas, including consecutive 1,200-yard rushing campaigns. Notably, his receiving numbers were excellent, placing him among the top five running backs in this class with a best-season reception share of at least 13% and a Breakout Score above 85.
-While his explosive run rate is below average, his pass protection skills, as graded by PFF, are a significant asset. This could facilitate early NFL playing time.
-Despite his solid overall profile, the primary concern is a lack of explosive running ability, potentially limiting him to a handcuff role rather than a starting position. His success hinges on a team utilizing his pass protection and receiving abilities, similar to his top comparable, Shane Vereen.</t>
-  </si>
-  <si>
-    <t>Ollie Gordon's 4.61 40-yard dash was mitigated by his significant 226-pound frame, resulting in a respectable Speed Score. He had a stellar 2023 season at Oklahoma State, leading the nation in rushing yards and winning the Doak Walker Award. 1  However, his production dipped in 2024.   
-Gordon's size and downhill running style suggest he can handle a substantial workload. However, his lack of elite speed and below-average explosive play rate limit his upside, making volume crucial for fantasy success.
-While players like James Conner and Rhamondre Stevenson have thrived with similar profiles, the depth of this running back class could lead to Gordon being part of a committee, limiting his immediate fantasy impact.
-He has the potential for high volume in the right situation, but it's uncertain if he'll command a significant workload early in his NFL career.</t>
-  </si>
-  <si>
-    <t>Trevor Etienne is projected to have a "Low Risk" Draft Capital Delta due to his strong ZAP Model evaluation, primarily driven by his pass-catching abilities.
-Despite his undersized 198-pound frame and limited collegiate workload (never exceeding 133 carries in a season), Etienne excels as a receiver. His top-season reception share ranks 10th in his class, and his Breakout Score is 11th.
-However, his yards per team play rate never exceeded 1.25, reflecting his limited rushing volume. Notably, his best-season yards per team play is among the lowest in his class.
-Despite this, historically, running backs with similar profiles—high Breakout Scores but low yards per team play—have found success as receivers in the NFL. Examples include Josh Jacobs, Tony Pollard, and James Cook.
-Etienne's NFL role is likely as a pass-catching back, not a high-volume rusher. He's dynamic with the ball and projects as valuable PPR depth, even if he doesn't reach his brother's fantasy heights.</t>
-  </si>
-  <si>
-    <t>Brashard Smith's unique journey from wide receiver at Miami to running back at SMU makes him an intriguing prospect.
-* **Transition and Production:** He excelled in his single season as a running back, rushing for 1,332 yards and showcasing explosive speed with a sub-4.4 40-yard dash.
-* **Comparison to Tyrone Tracy:** While similar in position change, Smith is smaller (194 pounds) than Tracy (209 pounds) and has less running back experience.
-* **Size Concerns:** Historically, smaller running backs (under 200 pounds) rarely command high rushing workloads in the NFL.
-* **Projected Role:** Smith is likely to begin his NFL career as a situational or mismatch player, leveraging his speed and agility.
-* **Fantasy Outlook:** He's projected as a bench stash, with potential for more if he develops, but his size limits his likely early career volume.</t>
-  </si>
-  <si>
-    <t>RJ Harvey presents an intriguing profile with a compact build similar to Jaylen Warren, but with a stronger production profile.
-Strong Production: He boasts a solid 11.1% top-year reception share and an impressive 2.23 max-season total yards per team play rate, ranking highly in his class.
-Combine Performance: His 4.40 40-yard dash resulted in a 109.4 Speed Score, highlighting his athleticism.1   
-Age Concerns: At 24, Harvey's age is a significant factor. He began as a quarterback at Virginia in 2019, transferred to UCF, and faced setbacks including the pandemic and an ACL tear.
-Historical Context: Historically, 24-year-old running back prospects have not yielded consistent, long-term fantasy success. Ray Davis and Tyrone Tracy are recent examples, but their NFL outcomes are yet to be determined.
-Fantasy Outlook: Harvey's production and athleticism are appealing, but his age introduces risk. He could be a valuable contributor, but his long-term fantasy potential is uncertain</t>
-  </si>
-  <si>
-    <t>LeQuint Allen boasts an exceptional receiving profile, ranking near the top of his class in reception share and Breakout Score. However, his rushing metrics are concerning.
-Receiving Dominance: He possesses elite receiving numbers, with a high reception share and Breakout Score, indicating significant pass-catching potential.
-Rushing Concerns: His tackle avoidance and yards after contact per attempt are below average, raising questions about his effectiveness as a rusher.
-Draft Capital Impact: His receiving profile is highly valuable, but it's heavily dependent on draft capital. A Day 3 selection would significantly diminish his fantasy prospects.
-Historical Precedent: Historically, running backs with similar receiving profiles but lower draft capital have had limited success, with Kyren Williams being a notable exception.
-Combine Uncertainty: Allen's decision to skip the combine leaves his speed and athleticism unknown, adding to the uncertainty surrounding his projection.
-Fantasy Outlook: Despite the rushing concerns, Allen's pass-catching prowess makes him an intriguing PPR prospect, especially given his young age. His fantasy value is heavily tied to his draft position.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Jarquez Hunter has the third-best Breakout Score in this year’s draft class. It seems wild 
 because he topped out at a 10.7% reception share at Auburn, which isn’t anything special. 
 His Breakout Score is high, though, because, as a Sophomore, Hunter had 224 receiving yards 
@@ -714,6 +590,130 @@
 reaching a 10% target share per game rate in one of their first three seasons. 
 Brooks can handle a lot of work -- he’s not a bad prospect -- but I’m not sure he’ll get 
 the opportunity to be a true three-down back in the NFL. </t>
+  </si>
+  <si>
+    <t>Raheim Rocket Sanders is a big, fast running back with good age-adjusted receiving production.Strengths:Size and speed combinationGood receiving productionHigh Breakout ScoreWeaknesses:Average explosivenessAverage tackle avoidanceOverall: Sanders has strong ZAP Model metrics.Concerns:His ultimate draft capital is a key factor in evaluating his potential.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tetairoa McMillan is an early-declare wide receiver with a lot of size, who gave Arizona solid production.   
+His Breakout Score is good, but not amazing, sitting at 83.1. His raw numbers in yards per team attempt were good, but they were brought down a bit when adjusted for the strength of the opponent.   
+His comparisons to Drake London don’t work well analytically, as London had a much better age-adjusted profile. Londons Breakout Score was elite. Profiles like Tee Higgins and Courtland Sutton make a lot more sense. They didn’t get the draft capital McMillan is likely to get, but their fantasy impacts have definitely been felt.   
+</t>
+  </si>
+  <si>
+    <t>The ZAP Model has seen nearly 60 wide receivers hit 14 or more PPR points per game in one of their first three seasons in the league.  Just 5 of those 60 did it with a best-season receiving yards per team pass attempt rate below 2.0.  One is Tyreek Hill, who we know is an outlier.  Another is Hunter Renfrow, who only gave us one good year.  The other three are Terry McLaurin, Nico Collins, and Ladd McConkey.    
+Matthew Golden’s best prorated receiving yards per team pass attempt figure was below 2.0.  It was 1.82, done in 2024, his third and final year of college football.  When we adjust for program strength, his top year in yards per team pass attempt is 2.28, not 1.82.  Those team strength adjustments are a key reason Golden’s Breakout Score is an OK-enough 51.4.    
+Golden started his college life at Houston, where he played two seasons and gave us some production.  Receiving yard per team pass attempt rates of 1.38 and 1.32 as a Freshman and Sophomore aren’t tragic.  His top season in yards per route run, per PFF, was 2.10.    
+Golden is probably going to get solid draft capital given his ability to create explosive plays.  Hes easy to like on film, and his most favorable comparable in the ZAP Model is Ladd McConkey.  So there are things working in his favor.  He’s just not close to a flawless prospect analytically.</t>
+  </si>
+  <si>
+    <t>When the initial NFL Combine list came out, the Heisman-winning Travis Hunter was only listed as a cornerback. That changed as we got closer to the combine, as he was added to the wide receiver list.  No one really knows how Hunter is going to be used at the next level.  Some believe that hell be a full-time corner who takes some snaps on offense.  If hes a part-time player on offense, then hell have a hard time living up to his ZAP score.    
+His production profile is kind of ordinary for a first-rounder.  His top year in receiving yards per team pass attempt came last season, where it was 2.61.  Thats a 20th percentile number among all first-round wide receivers since 2011.  His Breakout Score of 66.9 is a 15th percentile one compared to other first-rounders.  His career yards per route run looks slightly better, but, among first-round wide receivers over the last five seasons, its still below average.  His yards per route run rate was 2.51 last season.  There are 27 wide receivers in this years class who had a better rate than that during one of their collegiate seasons.    
+We can probably cut Hunter a bit of a break because, you know, he was playing on both offense and defense in college.  None of this is to take away from his insane gifts.  And, to be fair, a lot of evaluators who look solely at film think Hunter is as good as it gets.  If there were no restrictions here -- if we were simply assuming he would play wide receiver -- then Id more than likely be lower than the market on Hunter.  Its very possible that his metrics arent showing up well because, again, he did everything for Colorado.  But if were being completely objective, the predictive metrics we look at arent close to excellent.</t>
+  </si>
+  <si>
+    <t>No wide receiver in this years draft class has a higher best-season adjusted receiving yards per team pass attempt than Tre Harris.  Harris final season at Ole Miss was great.  A 60-catch, 1,030-yard campaign may not look like much, but he amassed that in just eight games.  That led to a (prorated) receiving yards per team pass attempt of 3.86.  Harris yards per route run last year was even crazier.  According to Pro Football Focus, he saw over five yards per route run.  Not only was that by far the highest in this years class, but it was the highest PFF has ever recorded from a Power Five wideout with 100 or more routes run.  That dates back to 2014.    
+As impressive as that is, it wasnt all butterflies and rainbows throughout Harris college career.  He started things off at Louisiana Tech, where he played three seasons.  There, he failed to really break out until his third year.  He then went to Ole Miss where he had back-to-back seasons of strong production, including his ridiculous 2024.    
+Were not usually looking for wide receivers who played five years of college ball.  Younger receivers give us better fantasy football odds.  But, because Harris numbers were so good at Ole Miss, he ended up with a pretty impressive 83.4 Breakout Score, a top-three number in the class.    
+Older players generally dont have upper-tier Breakout Scores in the model.  Since Breakout Score incorporates age, higher scores tend to correlate with at least average-aged prospects.    
+Harris is an exception.  Especially when you layer on projected draft capital.    
+If Harris gets drafted in the top-100 hes currently forecasted to go in Round 2 then hell become just the third wideout in ZAP Model history to get picked in the top-100 after turning 23 years old with a Breakout Score above 80. [cite: 4358, 4359, 480.9] The other two?  Sterling Shepard, who had a pretty decent career in the league, and Calvin Ridley.  NFL teams are always looking for perimeter players with decent size.  Harris has that.  And he might be pretty good, too.  Hes a higher-variance player to watch.    
+Sources and related content</t>
+  </si>
+  <si>
+    <t>Elic Ayomanor, a Canadian-born wide receiver with a unique high school path in the US, is entering the NFL draft after only two college seasons at Stanford. Despite a strong sophomore year with over 1,000 yards and a solid Breakout Score, his 2024 performance didnt significantly elevate his stats. Hes a prototypical X receiver with a large frame and impressive 4.44 40-yard dash time, excelling in downfield targets. While his college numbers are good, not exceptional, his physical attributes and the demand for his position could lead to decent draft capital.</t>
+  </si>
+  <si>
+    <t>The trend in football is shifting towards smaller, lighter wide receivers, but bigger players like Jayden Higgins stand out. At 6’4’’ and 214 pounds, Higgins combines size and smooth athleticism, which is rare for bigger receivers. Hes versatile, playing from the slot and all over the formation.
+Higgins stats improved at Iowa State after transferring from Eastern Kentucky, showing solid production. His Breakout Score of 74.7 and strong yards per route run highlight his potential. Historically, players with similar profiles have had decent success in the NFL. Higgins’ blend of size, versatility, and performance makes him an intriguing prospect.</t>
+  </si>
+  <si>
+    <t>Jaylin Noel, a versatile wide receiver from Iowa State, boasts above-average college stats, ranking in the 60-70th percentile among combine invitees. Primarily a slot receiver, he excelled in short-area targets and screens, evidenced by a low average depth of target (aDOT) early in his career. Despite this, he also demonstrated downfield capability, even surpassing his teammate Jayden Higgins in 20+ yard targets. Noels versatility extends to special teams, where he returned kicks and punts. His strong combine performance has boosted his draft stock, with some models projecting him higher than others.</t>
+  </si>
+  <si>
+    <t>DJ Giddens is an athletic running back with a strong profile.Strengths:Good 40-yard dash time.Impressive vertical and broad jumps.Solid production profile at Kansas State, including receiving ability.Stats:Speed Score over 110.Breakout Score over 75.High yards per team play rate.Comparison:Shares statistical traits with successful NFL running backs like Todd Gurley, Ezekiel Elliott, and others.Giddens profile suggests he has high potential, and his draft stock should be monitored.</t>
+  </si>
+  <si>
+    <t>Dylan Sampson, while possessing a 200-pound frame, doesnt align with the ideal size profile for high-end fantasy running backs. His production profile also doesnt compensate for this.
+Across his three seasons at Tennessee, Sampsons rushing volume increased, but his receiving numbers remained underwhelming, culminating in a best-season reception share of only 8.5% and a below-average Breakout Score of 45.0.
+His total yards per team play and yards after contact per attempt are also below average, and his tackle avoidance is considered ordinary. While he displayed some explosive runs, his absence at the combine leaves his speed untested.
+Sampsons potential NFL workload is a concern. Historically, coaches tend to limit the usage of 200-pound backs, and his limited receiving ability further diminishes his fantasy prospects. Consequently, he risks a negative Draft Capital Delta.</t>
+  </si>
+  <si>
+    <t>Jack Bechs NFL draft profile is intertwined with a recent personal tragedy: the loss of his brother, Tiger, in a New Orleans shooting. Bech honored his brother at the Senior Bowl, where he won MVP after scoring the game-winning touchdown. As a prospect, Bech had a promising freshman year at LSU, showing potential alongside future stars Brian Thomas Jr. and Malik Nabers. However, his role was primarily in the slot with short-range targets. After a quiet sophomore year, he transferred to TCU. His senior year was his most productive, but his overall analytical profile, including a below-average Breakout Score, is not particularly strong. Despite this, Bechs versatility, transitioning from a tight end/slot receiver to an X receiver, and his production against stiff competition at LSU, are noteworthy. While he has a favorable comparison to Michael Thomas, his overall draft projection is modest.</t>
+  </si>
+  <si>
+    <t>Devin Neals 4.58 40-yard dash time at the combine was underwhelming, failing to enhance his otherwise strong production profile. However, his overall ZAP Model score remains solid.
+Neal demonstrated consistent production across his four seasons at Kansas, including consecutive 1,200-yard rushing campaigns. Notably, his receiving numbers were excellent, placing him among the top five running backs in this class with a best-season reception share of at least 13% and a Breakout Score above 85.
+While his explosive run rate is below average, his pass protection skills, as graded by PFF, are a significant asset. This could facilitate early NFL playing time.
+Despite his solid overall profile, the primary concern is a lack of explosive running ability, potentially limiting him to a handcuff role rather than a starting position. His success hinges on a team utilizing his pass protection and receiving abilities, similar to his top comparable, Shane Vereen.</t>
+  </si>
+  <si>
+    <t>Xavier Restrepo, a slot receiver from Miami, lined up in the slot over 90% of his college routes, a high rate thats rare for top-100 draft picks. Historically, receivers with such high slot rates havent found much NFL success, but the sample size is small.
+Restrepos production was limited until his final two seasons, where he achieved adjusted receiving yards per team pass attempt rates around 2.40, resulting in a Breakout Score of 48.9. While film analysts praise his route-running and spatial awareness, his production profile is less impressive compared to successful NFL slot receivers like Josh Downs, Christian Kirk, and Cooper Kupp, who had significantly higher Breakout Scores.
+While Restrepo might find a role in the NFL, especially if he receives the projected draft capital, his ceiling as a fantasy football game-changer is questionable based on his college production.</t>
+  </si>
+  <si>
+    <t>Ollie Gordons 4.61 40-yard dash was mitigated by his significant 226-pound frame, resulting in a respectable Speed Score. He had a stellar 2023 season at Oklahoma State, leading the nation in rushing yards and winning the Doak Walker Award. 1  However, his production dipped in 2024.   
+Gordons size and downhill running style suggest he can handle a substantial workload. However, his lack of elite speed and below-average explosive play rate limit his upside, making volume crucial for fantasy success.
+While players like James Conner and Rhamondre Stevenson have thrived with similar profiles, the depth of this running back class could lead to Gordon being part of a committee, limiting his immediate fantasy impact.
+He has the potential for high volume in the right situation, but its uncertain if hell command a significant workload early in his NFL career.</t>
+  </si>
+  <si>
+    <t>RJ Harvey presents an intriguing profile with a compact build similar to Jaylen Warren, but with a stronger production profile.
+Strong Production: He boasts a solid 11.1% top-year reception share and an impressive 2.23 max-season total yards per team play rate, ranking highly in his class.
+Combine Performance: His 4.40 40-yard dash resulted in a 109.4 Speed Score, highlighting his athleticism.1   
+Age Concerns: At 24, Harveys age is a significant factor. He began as a quarterback at Virginia in 2019, transferred to UCF, and faced setbacks including the pandemic and an ACL tear.
+Historical Context: Historically, 24-year-old running back prospects have not yielded consistent, long-term fantasy success. Ray Davis and Tyrone Tracy are recent examples, but their NFL outcomes are yet to be determined.
+Fantasy Outlook: Harveys production and athleticism are appealing, but his age introduces risk. He could be a valuable contributor, but his long-term fantasy potential is uncertain</t>
+  </si>
+  <si>
+    <t>Trevor Etienne is projected to have a Low Risk Draft Capital Delta due to his strong ZAP Model evaluation, primarily driven by his pass-catching abilities.
+Despite his undersized 198-pound frame and limited collegiate workload (never exceeding 133 carries in a season), Etienne excels as a receiver. His top-season reception share ranks 10th in his class, and his Breakout Score is 11th.
+However, his yards per team play rate never exceeded 1.25, reflecting his limited rushing volume. Notably, his best-season yards per team play is among the lowest in his class.
+Despite this, historically, running backs with similar profiles—high Breakout Scores but low yards per team play—have found success as receivers in the NFL. Examples include Josh Jacobs, Tony Pollard, and James Cook.
+Etiennes NFL role is likely as a pass-catching back, not a high-volume rusher. Hes dynamic with the ball and projects as valuable PPR depth, even if he doesnt reach his brothers fantasy heights.</t>
+  </si>
+  <si>
+    <t>Ricky White boasts impressive raw production numbers, including high yards per route run and receiving yards per team pass attempt. However, these stats are inflated by the context of his competition at UNLV, in the Mountain West Conference.
+After transferring from Michigan State, where he played behind NFL-caliber receivers, White excelled at UNLV. While his raw numbers are strong, the ZAP Models adjustments for age and opponent strength result in a Breakout Score of 45.2. This creates a rare profile: a player with high raw production but a low adjusted score.
+Historically, players with this profile have had mixed results, with John Brown being a notable success and Christian Watson still developing. This suggests that Whites potential is uncertain.
+As a fantasy analyst, the takeaway is to monitor Whites draft capital and landing spot closely. While his raw numbers are enticing, the adjusted metrics suggest caution. Hes a player with high potential but also significant risk, and his fantasy value will depend heavily on his NFL opportunity. Avoid overpaying for him based on his raw college stats alone.</t>
+  </si>
+  <si>
+    <t>Savion Williams, a physically imposing 64, 220+ pound wide receiver from TCU, presents a unique profile due to his dual-threat ability as both a receiver and rusher. While his receiving production was notably low, with the worst adjusted receiving yards per team pass attempt rate in his draft class and a zero Breakout Score, his rushing stats are eye-catching. He recorded 51 carries for 322 yards and 6 touchdowns in his final college season. The ZAP Model values his versatility, particularly his rushing contribution, which boosts his overall evaluation. However, the model also acknowledges the significant risk associated with his poor receiving profile. Historically, wide receivers drafted in the top 100 without a Breakout Score have generally underperformed, with Terry McLaurin being a notable exception. Despite the analytical concerns, Williamss unique skill set could make him an intriguing Day 2 draft pick, offering a high ceiling if he lands in the right offensive system.</t>
+  </si>
+  <si>
+    <t>LeQuint Allen boasts an exceptional receiving profile, ranking near the top of his class in reception share and Breakout Score. However, his rushing metrics are concerning.
+Receiving Dominance: He possesses elite receiving numbers, with a high reception share and Breakout Score, indicating significant pass-catching potential.
+Rushing Concerns: His tackle avoidance and yards after contact per attempt are below average, raising questions about his effectiveness as a rusher.
+Draft Capital Impact: His receiving profile is highly valuable, but its heavily dependent on draft capital. A Day 3 selection would significantly diminish his fantasy prospects.
+Historical Precedent: Historically, running backs with similar receiving profiles but lower draft capital have had limited success, with Kyren Williams being a notable exception.
+Combine Uncertainty: Allens decision to skip the combine leaves his speed and athleticism unknown, adding to the uncertainty surrounding his projection.
+Fantasy Outlook: Despite the rushing concerns, Allens pass-catching prowess makes him an intriguing PPR prospect, especially given his young age. His fantasy value is heavily tied to his draft position.</t>
+  </si>
+  <si>
+    <t>Tez Johnson, at 154 pounds, is one of the lightest wide receiver prospects in recent NFL draft history. While smaller receivers have found success in the NFL, Johnsons size, combined with a potentially poor combine performance, raises concerns about his draft capital and fantasy potential. Historically, only a few sub-170-pound receivers have achieved significant fantasy production, and those players generally had stronger production profiles and better draft capital than Johnson.
+Johnsons college career spanned five years, with his most productive seasons at Oregon, where he posted impressive yards per route run numbers. However, his receiving yards per team pass attempt were more moderate.
+While Johnsons yards per route run is a positive indicator, similar to recent successes like Ladd McConkey and Puka Nacua, his lack of experience playing outside the slot limits his versatility compared to other successful small receivers.
+As a fantasy analyst, Johnsons size and limited perimeter experience suggest a lower ceiling. While he might find a role in the NFL, the odds of him becoming a high-end fantasy asset are lower than those of other small, but more versatile, receivers. Monitor his draft capital closely, but temper expectations.</t>
+  </si>
+  <si>
+    <t>Brashard Smiths unique journey from wide receiver at Miami to running back at SMU makes him an intriguing prospect.
+* **Transition and Production:** He excelled in his single season as a running back, rushing for 1,332 yards and showcasing explosive speed with a sub-4.4 40-yard dash.
+* **Comparison to Tyrone Tracy:** While similar in position change, Smith is smaller (194 pounds) than Tracy (209 pounds) and has less running back experience.
+* **Size Concerns:** Historically, smaller running backs (under 200 pounds) rarely command high rushing workloads in the NFL.
+* **Projected Role:** Smith is likely to begin his NFL career as a situational or mismatch player, leveraging his speed and agility.
+* **Fantasy Outlook:** Hes projected as a bench stash, with potential for more if he develops, but his size limits his likely early career volume.</t>
+  </si>
+  <si>
+    <t>Tai Felton, despite his low BMI, excels at forcing missed tackles and generating yards after the catch, ranking highly in both categories. However, his overall production profile is average, with a top-season receiving yards per team pass attempt of 2.28 and a Breakout Score of 56.3.
+Concerns exist about his play strength translating to the NFL, and his statistical comparisons are to players with similar builds who have struggled. His 4.37 speed is a potential asset, but relying solely on speed for NFL success is risky.
+Overall, Feltons profile is unremarkable, leading the ZAP Model to project him as a benchwarmer. As a fantasy analyst, he presents a low-ceiling prospect with limited upside.</t>
+  </si>
+  <si>
+    <t>Nick Nash, a former quarterback turned wide receiver, had a remarkable 2024 season at San Jose State, winning the college football triple crown in receptions, receiving yards, and receiving touchdowns. 1  However, his raw production needs context.   
+Despite his impressive raw numbers, his adjusted metrics, such as receiving yards per team pass attempt (2.71) and yards per route run (2.71), are merely average compared to other combine invitees. His age (almost 25) and the level of competition in the Mountain West Conference further temper his evaluation. His transition from quarterback to wide receiver is unique, but his Breakout Score of zero reflects the challenges posed by his age and program strength. While his 2024 season was undeniably productive, especially against larger programs, the raw numbers dont paint the full picture. As a fantasy analyst, Nashs size and recent success are intriguing, but his advanced age and adjusted metrics suggest caution. Hes a developmental prospect with a potentially limited ceiling, and his raw stats should be viewed with skepticism.</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1098,7 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1180,7 +1180,7 @@
         <v>211</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -1215,7 +1215,7 @@
         <v>221</v>
       </c>
       <c r="K3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
@@ -1241,7 +1241,7 @@
         <v>62</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>71</v>
@@ -1250,7 +1250,7 @@
         <v>219</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="174" x14ac:dyDescent="0.35">
@@ -1285,7 +1285,7 @@
         <v>206</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="348" x14ac:dyDescent="0.35">
@@ -1320,7 +1320,7 @@
         <v>202</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="174" x14ac:dyDescent="0.35">
@@ -1355,7 +1355,7 @@
         <v>202</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="203" x14ac:dyDescent="0.35">
@@ -1390,7 +1390,7 @@
         <v>224</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="203" x14ac:dyDescent="0.35">
@@ -1425,7 +1425,7 @@
         <v>221</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
@@ -1460,7 +1460,7 @@
         <v>191</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1512,7 +1512,7 @@
         <v>188</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
@@ -1547,7 +1547,7 @@
         <v>205</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1599,7 +1599,7 @@
         <v>219</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
@@ -1634,7 +1634,7 @@
         <v>206</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
@@ -1669,7 +1669,7 @@
         <v>180</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="145" x14ac:dyDescent="0.35">
@@ -1704,7 +1704,7 @@
         <v>214</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
@@ -1739,7 +1739,7 @@
         <v>206</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -1791,7 +1791,7 @@
         <v>194</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -1826,7 +1826,7 @@
         <v>212</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -1878,7 +1878,7 @@
         <v>205</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -1930,7 +1930,7 @@
         <v>200</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
@@ -1965,7 +1965,7 @@
         <v>214</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="232" x14ac:dyDescent="0.35">
@@ -2035,7 +2035,7 @@
         <v>196</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="203" x14ac:dyDescent="0.35">
@@ -2070,7 +2070,7 @@
         <v>209</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
@@ -2105,7 +2105,7 @@
         <v>226</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -2174,7 +2174,7 @@
         <v>217</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
@@ -2209,7 +2209,7 @@
         <v>205</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="348" x14ac:dyDescent="0.35">
@@ -2244,7 +2244,7 @@
         <v>204</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -2296,7 +2296,7 @@
         <v>198</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="261" x14ac:dyDescent="0.35">
@@ -2331,7 +2331,7 @@
         <v>184</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="174" x14ac:dyDescent="0.35">
@@ -2366,7 +2366,7 @@
         <v>222</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="246.5" x14ac:dyDescent="0.35">
@@ -2401,7 +2401,7 @@
         <v>204</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="232" x14ac:dyDescent="0.35">
@@ -2436,7 +2436,7 @@
         <v>154</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
@@ -2471,7 +2471,7 @@
         <v>194</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="377" x14ac:dyDescent="0.35">
@@ -2506,7 +2506,7 @@
         <v>217</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="174" x14ac:dyDescent="0.35">
@@ -2541,7 +2541,7 @@
         <v>183</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
@@ -2593,7 +2593,7 @@
         <v>212</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
@@ -2628,7 +2628,7 @@
         <v>204</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="203" x14ac:dyDescent="0.35">
@@ -2663,7 +2663,7 @@
         <v>203</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
@@ -2671,7 +2671,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
@@ -2689,7 +2689,7 @@
         <v>83</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>99</v>
@@ -2698,7 +2698,7 @@
         <v>214</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>